<commit_message>
v6 now runs for all countries
</commit_message>
<xml_diff>
--- a/SDG Financing Simplified model (Egypt)/Parameter Estimation v1.xlsx
+++ b/SDG Financing Simplified model (Egypt)/Parameter Estimation v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Wi2050\SDG Financing Simplified model (Egypt)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3580E08D-6BDD-4D48-9385-5EE14D2BD571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7EB08B3-F85F-47DD-8340-05D4E387F7AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32505" yWindow="1830" windowWidth="17250" windowHeight="9945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimization0" sheetId="5" r:id="rId1"/>
@@ -263,7 +263,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="54">
   <si>
     <t>kre0</t>
   </si>
@@ -423,6 +423,9 @@
   <si>
     <t>Let the algorithm decide how to split among ben and bk, with utilization rates, unemployment rate, and effective labor scaling</t>
   </si>
+  <si>
+    <t>starting mpk</t>
+  </si>
 </sst>
 </file>
 
@@ -431,11 +434,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -641,40 +651,41 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -899,10 +910,10 @@
   <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:U24"/>
+  <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -912,12 +923,12 @@
     <col min="17" max="16384" width="14.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="24" t="s">
         <v>10</v>
       </c>
@@ -969,31 +980,35 @@
       <c r="Q2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="14" t="s">
+      <c r="R2" s="6"/>
+      <c r="S2" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="T2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="14" t="s">
+      <c r="U2" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="U2" s="14" t="s">
+      <c r="V2" s="14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="18">
-        <f>G3*($B$15)^F3</f>
-        <v>1.5483328821615816</v>
+        <f t="shared" ref="B3:B12" si="0">G3*($B$15)^F3</f>
+        <v>1.5483328783485584</v>
       </c>
       <c r="C3" s="18">
         <f>(1-E3-F3)*$B$16</f>
-        <v>0.23120573103504574</v>
+        <v>0.23120573017937088</v>
       </c>
       <c r="D3" s="20">
         <f>(1-E3-F3)*(1-$B$16)</f>
-        <v>0.17436426896495424</v>
+        <v>0.17436426982062911</v>
       </c>
       <c r="E3" s="3">
         <v>0.06</v>
@@ -1002,8 +1017,8 @@
         <v>0.53442999999999996</v>
       </c>
       <c r="G3" s="15">
-        <f t="shared" ref="G3:G12" si="0">P3/O3</f>
-        <v>1.5483328821615816</v>
+        <f t="shared" ref="G3:G12" si="1">P3/O3</f>
+        <v>1.5483328783485584</v>
       </c>
       <c r="H3" s="3">
         <v>0.81218433380126998</v>
@@ -1024,48 +1039,56 @@
         <v>93.811000000000007</v>
       </c>
       <c r="N3" s="4">
-        <f t="shared" ref="N3:N12" si="1">M3*$B$15</f>
+        <f t="shared" ref="N3:N12" si="2">M3*$B$15</f>
         <v>93.811000000000007</v>
       </c>
       <c r="O3" s="4">
         <f>(I3+J3)^C3*(K3)^E3*(L3)^D3*(N3)^F3</f>
-        <v>206.93733898661898</v>
+        <v>206.93733949623606</v>
       </c>
       <c r="P3" s="3">
         <v>320.40788650000002</v>
       </c>
       <c r="Q3" s="7">
-        <f t="shared" ref="Q3:Q11" si="2">(P3-O3)^2</f>
-        <v>12875.565152986463</v>
-      </c>
-      <c r="S3" s="4">
-        <f>(I3+J3)^C3*(K3)^E3*(L3)^D3*(N3)^F3*G3</f>
+        <f>(P3-O3)^2</f>
+        <v>12875.565037333405</v>
+      </c>
+      <c r="R3" s="7">
+        <f>P3-0.05*SUM(I3:L3)</f>
+        <v>150.45038650000004</v>
+      </c>
+      <c r="S3" s="2">
+        <f>B3*P3/(SUM(I3:L3))*(1-F3)</f>
+        <v>6.7948862566212992E-2</v>
+      </c>
+      <c r="T3" s="4">
+        <f t="shared" ref="T3:T12" si="3">(I3+J3)^C3*(K3)^E3*(L3)^D3*(N3)^F3*G3</f>
         <v>320.40788650000002</v>
       </c>
-      <c r="T3" s="4">
-        <f>(I3+J3)^C3*(K3)^E3*(L3)^D3*(M3)^F3*B3</f>
+      <c r="U3" s="4">
+        <f t="shared" ref="U3:U12" si="4">(I3+J3)^C3*(K3)^E3*(L3)^D3*(M3)^F3*B3</f>
         <v>320.40788650000002</v>
       </c>
-      <c r="U3" s="2" t="b">
-        <f t="shared" ref="U3:U12" si="3">IF(AND(P3=S3,S3=T3),TRUE, FALSE)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V3" s="2" t="b">
+        <f t="shared" ref="V3:V12" si="5">IF(AND(P3=T3,T3=U3),TRUE, FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="18">
-        <f>G4*($B$15)^F4</f>
-        <v>2.7411442183001893</v>
+        <f t="shared" si="0"/>
+        <v>2.741144212850152</v>
       </c>
       <c r="C4" s="18">
-        <f t="shared" ref="C4:C12" si="4">(1-E4-F4)*$B$16</f>
-        <v>0.16308734752202059</v>
+        <f t="shared" ref="C4:C12" si="6">(1-E4-F4)*$B$16</f>
+        <v>0.16308734691844667</v>
       </c>
       <c r="D4" s="20">
-        <f t="shared" ref="D4:D12" si="5">(1-E4-F4)*(1-$B$16)</f>
-        <v>0.12299265247797941</v>
+        <f t="shared" ref="D4:D12" si="7">(1-E4-F4)*(1-$B$16)</f>
+        <v>0.12299265308155331</v>
       </c>
       <c r="E4" s="3">
         <v>0.13</v>
@@ -1074,8 +1097,8 @@
         <v>0.58391999999999999</v>
       </c>
       <c r="G4" s="15">
-        <f t="shared" si="0"/>
-        <v>2.7411442183001893</v>
+        <f t="shared" si="1"/>
+        <v>2.741144212850152</v>
       </c>
       <c r="H4" s="3">
         <v>0.36648318171501199</v>
@@ -1096,48 +1119,56 @@
         <v>0.622</v>
       </c>
       <c r="N4" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.622</v>
       </c>
       <c r="O4" s="4">
-        <f>(I4+J4)^C4*(K4)^E4*(L4)^D4*(N4)^F4</f>
-        <v>1.4002872480676056</v>
+        <f t="shared" ref="O4:O12" si="8">(I4+J4)^C4*(K4)^E4*(L4)^D4*(N4)^F4</f>
+        <v>1.400287250851705</v>
       </c>
       <c r="P4" s="3">
         <v>3.8383892940000002</v>
       </c>
       <c r="Q4" s="7">
-        <f t="shared" si="2"/>
-        <v>5.9443415863797284</v>
-      </c>
-      <c r="S4" s="4">
-        <f>(I4+J4)^C4*(K4)^E4*(L4)^D4*(N4)^F4*G4</f>
+        <f t="shared" ref="Q4:Q11" si="9">(P4-O4)^2</f>
+        <v>5.944341572803892</v>
+      </c>
+      <c r="R4" s="7">
+        <f t="shared" ref="R4:R12" si="10">P4-0.05*SUM(I4:L4)</f>
+        <v>2.1394105828000001</v>
+      </c>
+      <c r="S4" s="2">
+        <f t="shared" ref="S4:S12" si="11">B4*P4/(SUM(I4:L4))*(1-F4)</f>
+        <v>0.12883676513992834</v>
+      </c>
+      <c r="T4" s="4">
+        <f t="shared" si="3"/>
         <v>3.8383892940000002</v>
       </c>
-      <c r="T4" s="4">
-        <f>(I4+J4)^C4*(K4)^E4*(L4)^D4*(M4)^F4*B4</f>
+      <c r="U4" s="4">
+        <f t="shared" si="4"/>
         <v>3.8383892940000002</v>
       </c>
-      <c r="U4" s="2" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V4" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="18">
-        <f>G5*($B$15)^F5</f>
-        <v>1.5405410498506715</v>
+        <f t="shared" si="0"/>
+        <v>1.5405410439401956</v>
       </c>
       <c r="C5" s="18">
-        <f t="shared" si="4"/>
-        <v>0.2644069583829291</v>
+        <f t="shared" si="6"/>
+        <v>0.26440695740437903</v>
       </c>
       <c r="D5" s="20">
-        <f t="shared" si="5"/>
-        <v>0.19940304161707084</v>
+        <f t="shared" si="7"/>
+        <v>0.19940304259562092</v>
       </c>
       <c r="E5" s="3">
         <v>0.06</v>
@@ -1146,8 +1177,8 @@
         <v>0.47619</v>
       </c>
       <c r="G5" s="15">
-        <f t="shared" si="0"/>
-        <v>1.5405410498506715</v>
+        <f t="shared" si="1"/>
+        <v>1.5405410439401956</v>
       </c>
       <c r="H5" s="3">
         <v>0.62282443046569802</v>
@@ -1168,48 +1199,56 @@
         <v>4.6139999999999999</v>
       </c>
       <c r="N5" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.6139999999999999</v>
       </c>
       <c r="O5" s="4">
-        <f>(I5+J5)^C5*(K5)^E5*(L5)^D5*(N5)^F5</f>
-        <v>9.2424659838698631</v>
+        <f t="shared" si="8"/>
+        <v>9.2424660193297257</v>
       </c>
       <c r="P5" s="3">
         <v>14.238398249999999</v>
       </c>
       <c r="Q5" s="7">
-        <f t="shared" si="2"/>
-        <v>24.959339207760202</v>
-      </c>
-      <c r="S5" s="4">
-        <f>(I5+J5)^C5*(K5)^E5*(L5)^D5*(N5)^F5*G5</f>
+        <f t="shared" si="9"/>
+        <v>24.959338853450056</v>
+      </c>
+      <c r="R5" s="7">
+        <f t="shared" si="10"/>
+        <v>4.9465982509999993</v>
+      </c>
+      <c r="S5" s="2">
+        <f t="shared" si="11"/>
+        <v>6.1827024473022338E-2</v>
+      </c>
+      <c r="T5" s="4">
+        <f t="shared" si="3"/>
         <v>14.238398249999999</v>
       </c>
-      <c r="T5" s="4">
-        <f>(I5+J5)^C5*(K5)^E5*(L5)^D5*(M5)^F5*B5</f>
+      <c r="U5" s="4">
+        <f t="shared" si="4"/>
         <v>14.238398249999999</v>
       </c>
-      <c r="U5" s="2" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V5" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="18">
-        <f>G6*($B$15)^F6</f>
-        <v>0.64319424959898563</v>
+        <f t="shared" si="0"/>
+        <v>0.64319424769611344</v>
       </c>
       <c r="C6" s="18">
-        <f t="shared" si="4"/>
-        <v>0.29181051261735153</v>
+        <f t="shared" si="6"/>
+        <v>0.29181051153738291</v>
       </c>
       <c r="D6" s="20">
-        <f t="shared" si="5"/>
-        <v>0.22006948738264862</v>
+        <f t="shared" si="7"/>
+        <v>0.22006948846261717</v>
       </c>
       <c r="E6" s="3">
         <v>0.09</v>
@@ -1218,8 +1257,8 @@
         <v>0.39811999999999997</v>
       </c>
       <c r="G6" s="15">
-        <f t="shared" si="0"/>
-        <v>0.64319424959898563</v>
+        <f t="shared" si="1"/>
+        <v>0.64319424769611344</v>
       </c>
       <c r="H6" s="3">
         <v>0.3</v>
@@ -1240,48 +1279,56 @@
         <v>137.09299999999999</v>
       </c>
       <c r="N6" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>137.09299999999999</v>
       </c>
       <c r="O6" s="4">
-        <f>(I6+J6)^C6*(K6)^E6*(L6)^D6*(N6)^F6</f>
-        <v>68.880515206132642</v>
+        <f t="shared" si="8"/>
+        <v>68.880515409913713</v>
       </c>
       <c r="P6" s="3">
         <v>44.303551290000001</v>
       </c>
       <c r="Q6" s="7">
-        <f t="shared" si="2"/>
-        <v>604.02715533488583</v>
-      </c>
-      <c r="S6" s="4">
-        <f>(I6+J6)^C6*(K6)^E6*(L6)^D6*(N6)^F6*G6</f>
+        <f t="shared" si="9"/>
+        <v>604.02716535152592</v>
+      </c>
+      <c r="R6" s="7">
+        <f t="shared" si="10"/>
+        <v>30.823001290999997</v>
+      </c>
+      <c r="S6" s="2">
+        <f t="shared" si="11"/>
+        <v>6.3614042789716746E-2</v>
+      </c>
+      <c r="T6" s="4">
+        <f t="shared" si="3"/>
         <v>44.303551290000001</v>
       </c>
-      <c r="T6" s="4">
-        <f>(I6+J6)^C6*(K6)^E6*(L6)^D6*(M6)^F6*B6</f>
+      <c r="U6" s="4">
+        <f t="shared" si="4"/>
         <v>44.303551290000001</v>
       </c>
-      <c r="U6" s="2" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V6" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="18">
-        <f>G7*($B$15)^F7</f>
-        <v>1.156559589438954</v>
+        <f t="shared" si="0"/>
+        <v>1.1565595872382326</v>
       </c>
       <c r="C7" s="18">
-        <f t="shared" si="4"/>
-        <v>0.27518709590264884</v>
+        <f t="shared" si="6"/>
+        <v>0.27518709488420229</v>
       </c>
       <c r="D7" s="20">
-        <f t="shared" si="5"/>
-        <v>0.20753290409735117</v>
+        <f t="shared" si="7"/>
+        <v>0.20753290511579775</v>
       </c>
       <c r="E7" s="3">
         <v>0.09</v>
@@ -1290,8 +1337,8 @@
         <v>0.42727999999999999</v>
       </c>
       <c r="G7" s="15">
-        <f t="shared" si="0"/>
-        <v>1.156559589438954</v>
+        <f t="shared" si="1"/>
+        <v>1.1565595872382326</v>
       </c>
       <c r="H7" s="3">
         <v>1.1712350845336901</v>
@@ -1312,48 +1359,56 @@
         <v>195.71799999999999</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>195.71799999999999</v>
       </c>
       <c r="O7" s="4">
-        <f>(I7+J7)^C7*(K7)^E7*(L7)^D7*(N7)^F7</f>
-        <v>303.238602232446</v>
+        <f t="shared" si="8"/>
+        <v>303.2386028094536</v>
       </c>
       <c r="P7" s="3">
         <v>350.71351329999999</v>
       </c>
       <c r="Q7" s="7">
-        <f t="shared" si="2"/>
-        <v>2253.8671808721601</v>
-      </c>
-      <c r="S7" s="4">
-        <f>(I7+J7)^C7*(K7)^E7*(L7)^D7*(N7)^F7*G7</f>
-        <v>350.71351330000005</v>
+        <f t="shared" si="9"/>
+        <v>2253.8671260853921</v>
+      </c>
+      <c r="R7" s="7">
+        <f t="shared" si="10"/>
+        <v>258.83101328888887</v>
+      </c>
+      <c r="S7" s="2">
+        <f t="shared" si="11"/>
+        <v>0.12641542335175784</v>
       </c>
       <c r="T7" s="4">
-        <f>(I7+J7)^C7*(K7)^E7*(L7)^D7*(M7)^F7*B7</f>
-        <v>350.71351330000005</v>
-      </c>
-      <c r="U7" s="2" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>350.71351329999999</v>
+      </c>
+      <c r="U7" s="4">
+        <f t="shared" si="4"/>
+        <v>350.71351329999999</v>
+      </c>
+      <c r="V7" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>16</v>
       </c>
       <c r="B8" s="18">
-        <f>G8*($B$15)^F8</f>
-        <v>1.0607844053747184</v>
+        <f t="shared" si="0"/>
+        <v>1.0607844024556607</v>
       </c>
       <c r="C8" s="18">
-        <f t="shared" si="4"/>
-        <v>0.26852860800046346</v>
+        <f t="shared" si="6"/>
+        <v>0.26852860700665943</v>
       </c>
       <c r="D8" s="20">
-        <f t="shared" si="5"/>
-        <v>0.20251139199953658</v>
+        <f t="shared" si="7"/>
+        <v>0.20251139299334059</v>
       </c>
       <c r="E8" s="3">
         <v>0.11</v>
@@ -1362,8 +1417,8 @@
         <v>0.41896</v>
       </c>
       <c r="G8" s="15">
-        <f t="shared" si="0"/>
-        <v>1.0607844053747184</v>
+        <f t="shared" si="1"/>
+        <v>1.0607844024556607</v>
       </c>
       <c r="H8" s="3">
         <v>0.5</v>
@@ -1384,48 +1439,56 @@
         <v>52.981999999999999</v>
       </c>
       <c r="N8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52.981999999999999</v>
       </c>
       <c r="O8" s="4">
-        <f>(I8+J8)^C8*(K8)^E8*(L8)^D8*(N8)^F8</f>
-        <v>60.731799848851175</v>
+        <f t="shared" si="8"/>
+        <v>60.731800015972432</v>
       </c>
       <c r="P8" s="3">
         <v>64.423346190000004</v>
       </c>
       <c r="Q8" s="7">
-        <f t="shared" si="2"/>
-        <v>13.627514388849306</v>
-      </c>
-      <c r="S8" s="4">
-        <f>(I8+J8)^C8*(K8)^E8*(L8)^D8*(N8)^F8*G8</f>
+        <f t="shared" si="9"/>
+        <v>13.627513154977603</v>
+      </c>
+      <c r="R8" s="7">
+        <f t="shared" si="10"/>
+        <v>43.262996192000003</v>
+      </c>
+      <c r="S8" s="2">
+        <f t="shared" si="11"/>
+        <v>9.3826084434666765E-2</v>
+      </c>
+      <c r="T8" s="4">
+        <f t="shared" si="3"/>
         <v>64.423346190000004</v>
       </c>
-      <c r="T8" s="4">
-        <f>(I8+J8)^C8*(K8)^E8*(L8)^D8*(M8)^F8*B8</f>
+      <c r="U8" s="4">
+        <f t="shared" si="4"/>
         <v>64.423346190000004</v>
       </c>
-      <c r="U8" s="2" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V8" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="18">
-        <f>G9*($B$15)^F9</f>
-        <v>0.96437146973333499</v>
+        <f t="shared" si="0"/>
+        <v>0.96437146547702479</v>
       </c>
       <c r="C9" s="18">
-        <f t="shared" si="4"/>
-        <v>0.29105231151205124</v>
+        <f t="shared" si="6"/>
+        <v>0.29105231043488872</v>
       </c>
       <c r="D9" s="20">
-        <f t="shared" si="5"/>
-        <v>0.21949768848794882</v>
+        <f t="shared" si="7"/>
+        <v>0.21949768956511134</v>
       </c>
       <c r="E9" s="3">
         <v>0.09</v>
@@ -1434,8 +1497,8 @@
         <v>0.39945000000000003</v>
       </c>
       <c r="G9" s="15">
-        <f t="shared" si="0"/>
-        <v>0.96437146973333499</v>
+        <f t="shared" si="1"/>
+        <v>0.96437146547702479</v>
       </c>
       <c r="H9" s="3">
         <v>0.44486066699027998</v>
@@ -1456,48 +1519,56 @@
         <v>593.95699999999999</v>
       </c>
       <c r="N9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>593.95699999999999</v>
       </c>
       <c r="O9" s="4">
-        <f>(I9+J9)^C9*(K9)^E9*(L9)^D9*(N9)^F9</f>
-        <v>1057.6238244397994</v>
+        <f t="shared" si="8"/>
+        <v>1057.6238291076843</v>
       </c>
       <c r="P9" s="3">
         <v>1019.942242</v>
       </c>
       <c r="Q9" s="7">
-        <f t="shared" si="2"/>
-        <v>1419.9016551673985</v>
-      </c>
-      <c r="S9" s="4">
-        <f>(I9+J9)^C9*(K9)^E9*(L9)^D9*(N9)^F9*G9</f>
+        <f t="shared" si="9"/>
+        <v>1419.9020069540013</v>
+      </c>
+      <c r="R9" s="7">
+        <f t="shared" si="10"/>
+        <v>130.65224194374991</v>
+      </c>
+      <c r="S9" s="2">
+        <f t="shared" si="11"/>
+        <v>3.3212051102078873E-2</v>
+      </c>
+      <c r="T9" s="4">
+        <f t="shared" si="3"/>
         <v>1019.942242</v>
       </c>
-      <c r="T9" s="4">
-        <f>(I9+J9)^C9*(K9)^E9*(L9)^D9*(M9)^F9*B9</f>
+      <c r="U9" s="4">
+        <f t="shared" si="4"/>
         <v>1019.942242</v>
       </c>
-      <c r="U9" s="2" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V9" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="18">
-        <f>G10*($B$15)^F10</f>
-        <v>0.37595688404037308</v>
+        <f t="shared" si="0"/>
+        <v>0.37595688357743229</v>
       </c>
       <c r="C10" s="18">
-        <f t="shared" si="4"/>
-        <v>0.18099343527952436</v>
+        <f t="shared" si="6"/>
+        <v>0.18099343460968137</v>
       </c>
       <c r="D10" s="20">
-        <f t="shared" si="5"/>
-        <v>0.13649656472047569</v>
+        <f t="shared" si="7"/>
+        <v>0.13649656539031868</v>
       </c>
       <c r="E10" s="3">
         <v>0.1</v>
@@ -1506,8 +1577,8 @@
         <v>0.58250999999999997</v>
       </c>
       <c r="G10" s="15">
-        <f t="shared" si="0"/>
-        <v>0.37595688404037308</v>
+        <f t="shared" si="1"/>
+        <v>0.37595688357743229</v>
       </c>
       <c r="H10" s="3">
         <v>0.28394982218742398</v>
@@ -1528,48 +1599,56 @@
         <v>40.465000000000003</v>
       </c>
       <c r="N10" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40.465000000000003</v>
       </c>
       <c r="O10" s="4">
-        <f>(I10+J10)^C10*(K10)^E10*(L10)^D10*(N10)^F10</f>
-        <v>33.15087218528388</v>
+        <f t="shared" si="8"/>
+        <v>33.150872226104759</v>
       </c>
       <c r="P10" s="3">
         <v>12.463298610000001</v>
       </c>
       <c r="Q10" s="7">
-        <f t="shared" si="2"/>
-        <v>427.97570043278375</v>
-      </c>
-      <c r="S10" s="4">
-        <f>(I10+J10)^C10*(K10)^E10*(L10)^D10*(N10)^F10*G10</f>
+        <f t="shared" si="9"/>
+        <v>427.97570212175367</v>
+      </c>
+      <c r="R10" s="7">
+        <f t="shared" si="10"/>
+        <v>6.5961486100000002</v>
+      </c>
+      <c r="S10" s="2">
+        <f t="shared" si="11"/>
+        <v>1.6670933979905975E-2</v>
+      </c>
+      <c r="T10" s="4">
+        <f t="shared" si="3"/>
         <v>12.463298610000001</v>
       </c>
-      <c r="T10" s="4">
-        <f>(I10+J10)^C10*(K10)^E10*(L10)^D10*(M10)^F10*B10</f>
+      <c r="U10" s="4">
+        <f t="shared" si="4"/>
         <v>12.463298610000001</v>
       </c>
-      <c r="U10" s="2" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="V10" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="18">
-        <f>G11*($B$15)^F11</f>
-        <v>1.1733772783364189</v>
+        <f t="shared" si="0"/>
+        <v>1.1733772761314785</v>
       </c>
       <c r="C11" s="18">
-        <f t="shared" si="4"/>
-        <v>0.20167009248947854</v>
+        <f t="shared" si="6"/>
+        <v>0.20167009174311282</v>
       </c>
       <c r="D11" s="20">
-        <f t="shared" si="5"/>
-        <v>0.15208990751052154</v>
+        <f t="shared" si="7"/>
+        <v>0.15208990825688726</v>
       </c>
       <c r="E11" s="3">
         <v>0.09</v>
@@ -1578,8 +1657,8 @@
         <v>0.55623999999999996</v>
       </c>
       <c r="G11" s="15">
-        <f t="shared" si="0"/>
-        <v>1.1733772783364189</v>
+        <f t="shared" si="1"/>
+        <v>1.1733772761314785</v>
       </c>
       <c r="H11" s="3">
         <v>0.54299837350845304</v>
@@ -1600,48 +1679,56 @@
         <v>124.596</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>124.596</v>
       </c>
       <c r="O11" s="4">
-        <f>(I11+J11)^C11*(K11)^E11*(L11)^D11*(N11)^F11</f>
-        <v>229.31549363345854</v>
+        <f t="shared" si="8"/>
+        <v>229.31549406437452</v>
       </c>
       <c r="P11" s="3">
         <v>269.07358979999998</v>
       </c>
       <c r="Q11" s="7">
-        <f t="shared" si="2"/>
-        <v>1580.7062107879567</v>
-      </c>
-      <c r="S11" s="4">
-        <f>(I11+J11)^C11*(K11)^E11*(L11)^D11*(N11)^F11*G11</f>
+        <f t="shared" si="9"/>
+        <v>1580.7061765231595</v>
+      </c>
+      <c r="R11" s="7">
+        <f t="shared" si="10"/>
+        <v>124.43308979999995</v>
+      </c>
+      <c r="S11" s="2">
+        <f t="shared" si="11"/>
+        <v>4.8432511353810909E-2</v>
+      </c>
+      <c r="T11" s="4">
+        <f t="shared" si="3"/>
         <v>269.07358979999998</v>
       </c>
-      <c r="T11" s="4">
-        <f>(I11+J11)^C11*(K11)^E11*(L11)^D11*(M11)^F11*B11</f>
+      <c r="U11" s="4">
+        <f t="shared" si="4"/>
         <v>269.07358979999998</v>
       </c>
-      <c r="U11" s="2" t="b">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V11" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="21" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="22">
-        <f>G12*($B$15)^F12</f>
-        <v>2.3418570142599684</v>
+        <f t="shared" si="0"/>
+        <v>2.3418570100859708</v>
       </c>
       <c r="C12" s="22">
-        <f t="shared" si="4"/>
-        <v>0.12225850303961316</v>
+        <f t="shared" si="6"/>
+        <v>0.12225850258714371</v>
       </c>
       <c r="D12" s="23">
-        <f t="shared" si="5"/>
-        <v>9.220149696038682E-2</v>
+        <f t="shared" si="7"/>
+        <v>9.220149741285627E-2</v>
       </c>
       <c r="E12" s="3">
         <v>0.13</v>
@@ -1650,8 +1737,8 @@
         <v>0.65554000000000001</v>
       </c>
       <c r="G12" s="15">
-        <f t="shared" si="0"/>
-        <v>2.3418570142599684</v>
+        <f t="shared" si="1"/>
+        <v>2.3418570100859708</v>
       </c>
       <c r="H12" s="3">
         <v>0.51462882757186901</v>
@@ -1672,34 +1759,42 @@
         <v>134.20699999999999</v>
       </c>
       <c r="N12" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>134.20699999999999</v>
       </c>
       <c r="O12" s="4">
-        <f>(I12+J12)^C12*(K12)^E12*(L12)^D12*(N12)^F12</f>
-        <v>181.27698053937368</v>
+        <f t="shared" si="8"/>
+        <v>181.27698086247185</v>
       </c>
       <c r="P12" s="3">
         <v>424.52476840000003</v>
       </c>
       <c r="Q12" s="7">
         <f>(P12-O12)^2</f>
-        <v>59169.486299088276</v>
-      </c>
-      <c r="S12" s="4">
-        <f>(I12+J12)^C12*(K12)^E12*(L12)^D12*(N12)^F12*G12</f>
-        <v>424.52476840000003</v>
+        <v>59169.486141902453</v>
+      </c>
+      <c r="R12" s="7">
+        <f t="shared" si="10"/>
+        <v>268.75276840000004</v>
+      </c>
+      <c r="S12" s="2">
+        <f t="shared" si="11"/>
+        <v>0.10992154237047068</v>
       </c>
       <c r="T12" s="4">
-        <f>(I12+J12)^C12*(K12)^E12*(L12)^D12*(M12)^F12*B12</f>
-        <v>424.52476840000003</v>
-      </c>
-      <c r="U12" s="2" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>424.52476840000008</v>
+      </c>
+      <c r="U12" s="4">
+        <f t="shared" si="4"/>
+        <v>424.52476840000008</v>
+      </c>
+      <c r="V12" s="2" t="b">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="11"/>
       <c r="C13" s="4"/>
@@ -1716,8 +1811,10 @@
       <c r="N13" s="4"/>
       <c r="O13" s="3"/>
       <c r="P13" s="7"/>
-    </row>
-    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
+    </row>
+    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
@@ -1738,7 +1835,7 @@
       <c r="O14" s="3"/>
       <c r="P14" s="7"/>
     </row>
-    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>25</v>
       </c>
@@ -1759,12 +1856,12 @@
       <c r="O15" s="3"/>
       <c r="P15" s="7"/>
     </row>
-    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="10">
-        <v>0.57007601902272298</v>
+        <v>0.57007601691291487</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1786,7 +1883,7 @@
       </c>
       <c r="B17" s="4">
         <f>CORREL(O3:O12,P3:P12)</f>
-        <v>0.96361485640976241</v>
+        <v>0.96361485627157184</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1808,7 +1905,7 @@
       </c>
       <c r="B18" s="4">
         <f>CORREL(G3:G12,H3:H12)</f>
-        <v>8.4349253185432627E-2</v>
+        <v>8.4349253193680168E-2</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1864,7 +1961,7 @@
       </c>
       <c r="B21" s="4">
         <f>AVERAGE(G3:G12)</f>
-        <v>1.3546119041095195</v>
+        <v>1.3546119007800821</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1886,7 +1983,7 @@
       </c>
       <c r="B22" s="27">
         <f>AVERAGE(B3:B12)</f>
-        <v>1.3546119041095195</v>
+        <v>1.3546119007800821</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>44</v>
@@ -1897,7 +1994,7 @@
         <v>38</v>
       </c>
       <c r="B24" s="17">
-        <f>COUNTIF(U3:U12,"="&amp;TRUE)/10</f>
+        <f>COUNTIF(V3:V12,"="&amp;TRUE)/10</f>
         <v>1</v>
       </c>
     </row>
@@ -1914,7 +2011,7 @@
   <dimension ref="A1:V24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B9" activeCellId="1" sqref="H7 B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2977,8 +3074,8 @@
   </sheetPr>
   <dimension ref="A1:X27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3069,16 +3166,16 @@
         <v>12</v>
       </c>
       <c r="B3" s="18">
-        <f>G3*((1-P3)*$B$15)^F3</f>
-        <v>3.197336165001456</v>
+        <f>G3*((1-P3)^($B$17)*$B$15)^F3</f>
+        <v>1.7023065764741367</v>
       </c>
       <c r="C3" s="18">
         <f>(1-E3-F3)*$B$16</f>
-        <v>0.35514785081606554</v>
+        <v>0.19416085943728614</v>
       </c>
       <c r="D3" s="20">
         <f>(1-E3-F3)*(1-$B$16)</f>
-        <v>5.042214918393443E-2</v>
+        <v>0.21140914056271384</v>
       </c>
       <c r="E3" s="3">
         <v>0.06</v>
@@ -3088,7 +3185,7 @@
       </c>
       <c r="G3" s="15">
         <f>S3/R3</f>
-        <v>0.99344804310258572</v>
+        <v>1.7023065764741367</v>
       </c>
       <c r="H3" s="3">
         <v>0.81218433380126998</v>
@@ -3119,26 +3216,26 @@
       </c>
       <c r="Q3" s="4">
         <f t="shared" ref="Q3:Q12" si="0">O3*$B$15*(1-P3*$B$17)</f>
-        <v>835.85601000000008</v>
+        <v>93.811000000000007</v>
       </c>
       <c r="R3" s="4">
-        <f>(I3*K3+J3*L3)^C3*(M3)^E3*(N3)^D3*(Q3)^F3</f>
-        <v>322.52103038962247</v>
+        <f t="shared" ref="R3:R12" si="1">(I3*K3+J3*L3)^C3*(M3)^E3*(N3)^D3*(Q3)^F3</f>
+        <v>188.21984883806152</v>
       </c>
       <c r="S3" s="3">
         <v>320.40788650000002</v>
       </c>
       <c r="T3" s="7">
         <f>(S3-R3)^2</f>
-        <v>4.4653770982486947</v>
+        <v>17473.677300914071</v>
       </c>
       <c r="V3" s="4">
-        <f>G3*(I3*K3+J3*L3)^C3*(M3)^E3*(N3)^D3*(Q3)^F3</f>
+        <f t="shared" ref="V3:V12" si="2">G3*(I3*K3+J3*L3)^C3*(M3)^E3*(N3)^D3*(Q3)^F3</f>
         <v>320.40788650000007</v>
       </c>
       <c r="W3" s="4">
-        <f>B3*(I3*K3+J3*L3)^C3*(M3)^E3*(N3)^D3*(O3)^F3</f>
-        <v>320.4078864999999</v>
+        <f t="shared" ref="W3:W12" si="3">B3*(I3*K3+J3*L3)^C3*(M3)^E3*(N3)^D3*(O3)^F3</f>
+        <v>320.40788650000007</v>
       </c>
       <c r="X3" s="2" t="b">
         <f>IF(AND(S3=V3,V3=W3),TRUE, FALSE)</f>
@@ -3150,16 +3247,16 @@
         <v>9</v>
       </c>
       <c r="B4" s="18">
-        <f>G4*((1-P4)*$B$15)^F4</f>
-        <v>4.4617295722088564</v>
+        <f t="shared" ref="B4:B12" si="4">G4*((1-P4)^($B$17)*$B$15)^F4</f>
+        <v>2.8043899748075476</v>
       </c>
       <c r="C4" s="18">
-        <f t="shared" ref="C4:C12" si="1">(1-E4-F4)*$B$16</f>
-        <v>0.25051334458036845</v>
+        <f t="shared" ref="C4:C12" si="5">(1-E4-F4)*$B$16</f>
+        <v>0.13695672428389383</v>
       </c>
       <c r="D4" s="20">
-        <f t="shared" ref="D4:D12" si="2">(1-E4-F4)*(1-$B$16)</f>
-        <v>3.556665541963154E-2</v>
+        <f t="shared" ref="D4:D12" si="6">(1-E4-F4)*(1-$B$16)</f>
+        <v>0.14912327571610617</v>
       </c>
       <c r="E4" s="3">
         <v>0.13</v>
@@ -3168,8 +3265,8 @@
         <v>0.58391999999999999</v>
       </c>
       <c r="G4" s="15">
-        <f t="shared" ref="G4:G12" si="3">S4/R4</f>
-        <v>1.2401089884371326</v>
+        <f t="shared" ref="G4:G12" si="7">S4/R4</f>
+        <v>2.8043899748075476</v>
       </c>
       <c r="H4" s="3">
         <v>0.36648318171501199</v>
@@ -3200,29 +3297,29 @@
       </c>
       <c r="Q4" s="4">
         <f t="shared" si="0"/>
-        <v>5.5724980000000004</v>
+        <v>0.622</v>
       </c>
       <c r="R4" s="4">
-        <f>(I4*K4+J4*L4)^C4*(M4)^E4*(N4)^D4*(Q4)^F4</f>
-        <v>3.0952031876144952</v>
+        <f t="shared" si="1"/>
+        <v>1.368707393936327</v>
       </c>
       <c r="S4" s="3">
         <v>3.8383892940000002</v>
       </c>
       <c r="T4" s="7">
-        <f t="shared" ref="T4:T12" si="4">(S4-R4)^2</f>
-        <v>0.55232558872444715</v>
+        <f t="shared" ref="T4:T12" si="8">(S4-R4)^2</f>
+        <v>6.0993286875021138</v>
       </c>
       <c r="V4" s="4">
-        <f>G4*(I4*K4+J4*L4)^C4*(M4)^E4*(N4)^D4*(Q4)^F4</f>
-        <v>3.8383892940000002</v>
+        <f t="shared" si="2"/>
+        <v>3.8383892939999997</v>
       </c>
       <c r="W4" s="4">
-        <f>B4*(I4*K4+J4*L4)^C4*(M4)^E4*(N4)^D4*(O4)^F4</f>
+        <f t="shared" si="3"/>
         <v>3.8383892939999997</v>
       </c>
       <c r="X4" s="2" t="b">
-        <f t="shared" ref="X4:X12" si="5">IF(AND(S4=V4,V4=W4),TRUE, FALSE)</f>
+        <f t="shared" ref="X4:X12" si="9">IF(AND(S4=V4,V4=W4),TRUE, FALSE)</f>
         <v>1</v>
       </c>
     </row>
@@ -3231,16 +3328,16 @@
         <v>13</v>
       </c>
       <c r="B5" s="18">
-        <f>G5*((1-P5)*$B$15)^F5</f>
-        <v>3.8459338599676451</v>
+        <f t="shared" si="4"/>
+        <v>1.5878606210228356</v>
       </c>
       <c r="C5" s="18">
-        <f t="shared" si="1"/>
-        <v>0.40614721179327701</v>
+        <f t="shared" si="5"/>
+        <v>0.22204242970537189</v>
       </c>
       <c r="D5" s="20">
-        <f t="shared" si="2"/>
-        <v>5.7662788206722951E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.24176757029462803</v>
       </c>
       <c r="E5" s="3">
         <v>0.06</v>
@@ -3249,8 +3346,8 @@
         <v>0.47619</v>
       </c>
       <c r="G5" s="15">
-        <f t="shared" si="3"/>
-        <v>1.4577099120251724</v>
+        <f t="shared" si="7"/>
+        <v>1.5878606210228356</v>
       </c>
       <c r="H5" s="3">
         <v>0.62282443046569802</v>
@@ -3281,29 +3378,29 @@
       </c>
       <c r="Q5" s="4">
         <f t="shared" si="0"/>
-        <v>35.389380000000003</v>
+        <v>4.6139999999999999</v>
       </c>
       <c r="R5" s="4">
-        <f>(I5*K5+J5*L5)^C5*(M5)^E5*(N5)^D5*(Q5)^F5</f>
-        <v>9.7676486470609412</v>
+        <f t="shared" si="1"/>
+        <v>8.9670327870642694</v>
       </c>
       <c r="S5" s="3">
         <v>14.238398249999999</v>
       </c>
       <c r="T5" s="7">
-        <f t="shared" si="4"/>
-        <v>19.987602012179746</v>
+        <f t="shared" si="8"/>
+        <v>27.787293843831623</v>
       </c>
       <c r="V5" s="4">
-        <f>G5*(I5*K5+J5*L5)^C5*(M5)^E5*(N5)^D5*(Q5)^F5</f>
-        <v>14.238398249999999</v>
+        <f t="shared" si="2"/>
+        <v>14.238398250000001</v>
       </c>
       <c r="W5" s="4">
-        <f>B5*(I5*K5+J5*L5)^C5*(M5)^E5*(N5)^D5*(O5)^F5</f>
-        <v>14.238398249999994</v>
+        <f t="shared" si="3"/>
+        <v>14.238398250000001</v>
       </c>
       <c r="X5" s="2" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -3312,16 +3409,16 @@
         <v>14</v>
       </c>
       <c r="B6" s="18">
-        <f>G6*((1-P6)*$B$15)^F6</f>
-        <v>1.4777020577307953</v>
+        <f t="shared" si="4"/>
+        <v>0.70544917162533272</v>
       </c>
       <c r="C6" s="18">
-        <f t="shared" si="1"/>
-        <v>0.4482409494679776</v>
+        <f t="shared" si="5"/>
+        <v>0.24505525736311376</v>
       </c>
       <c r="D6" s="20">
-        <f t="shared" si="2"/>
-        <v>6.3639050532022498E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.26682474263688633</v>
       </c>
       <c r="E6" s="3">
         <v>0.09</v>
@@ -3330,8 +3427,8 @@
         <v>0.39811999999999997</v>
       </c>
       <c r="G6" s="15">
-        <f t="shared" si="3"/>
-        <v>0.60411544453609567</v>
+        <f t="shared" si="7"/>
+        <v>0.70544917162533272</v>
       </c>
       <c r="H6" s="3">
         <v>0.3</v>
@@ -3362,29 +3459,29 @@
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="0"/>
-        <v>1296.4885009999998</v>
+        <v>137.09299999999999</v>
       </c>
       <c r="R6" s="4">
-        <f>(I6*K6+J6*L6)^C6*(M6)^E6*(N6)^D6*(Q6)^F6</f>
-        <v>73.336233481037709</v>
+        <f t="shared" si="1"/>
+        <v>62.801904193786228</v>
       </c>
       <c r="S6" s="3">
         <v>44.303551290000001</v>
       </c>
       <c r="T6" s="7">
-        <f t="shared" si="4"/>
-        <v>842.89663520579802</v>
+        <f t="shared" si="8"/>
+        <v>342.18906015301633</v>
       </c>
       <c r="V6" s="4">
-        <f>G6*(I6*K6+J6*L6)^C6*(M6)^E6*(N6)^D6*(Q6)^F6</f>
+        <f t="shared" si="2"/>
         <v>44.303551290000009</v>
       </c>
       <c r="W6" s="4">
-        <f>B6*(I6*K6+J6*L6)^C6*(M6)^E6*(N6)^D6*(O6)^F6</f>
-        <v>44.303551290000001</v>
+        <f t="shared" si="3"/>
+        <v>44.303551290000009</v>
       </c>
       <c r="X6" s="2" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -3393,16 +3490,16 @@
         <v>15</v>
       </c>
       <c r="B7" s="18">
-        <f>G7*((1-P7)*$B$15)^F7</f>
-        <v>2.2851856448272163</v>
+        <f t="shared" si="4"/>
+        <v>1.3293547635732779</v>
       </c>
       <c r="C7" s="18">
-        <f t="shared" si="1"/>
-        <v>0.42270624194573364</v>
+        <f t="shared" si="5"/>
+        <v>0.23109532279894165</v>
       </c>
       <c r="D7" s="20">
-        <f t="shared" si="2"/>
-        <v>6.0013758054266418E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.25162467720105836</v>
       </c>
       <c r="E7" s="3">
         <v>0.09</v>
@@ -3411,8 +3508,8 @@
         <v>0.42727999999999999</v>
       </c>
       <c r="G7" s="15">
-        <f t="shared" si="3"/>
-        <v>0.88207921360116393</v>
+        <f t="shared" si="7"/>
+        <v>1.3293547635732779</v>
       </c>
       <c r="H7" s="3">
         <v>1.1712350845336901</v>
@@ -3443,29 +3540,29 @@
       </c>
       <c r="Q7" s="4">
         <f t="shared" si="0"/>
-        <v>1816.26304</v>
+        <v>195.71799999999999</v>
       </c>
       <c r="R7" s="4">
-        <f>(I7*K7+J7*L7)^C7*(M7)^E7*(N7)^D7*(Q7)^F7</f>
-        <v>397.59865995275192</v>
+        <f t="shared" si="1"/>
+        <v>263.82236172779744</v>
       </c>
       <c r="S7" s="3">
         <v>350.71351329999999</v>
       </c>
       <c r="T7" s="7">
-        <f t="shared" si="4"/>
-        <v>2198.2169766500551</v>
+        <f t="shared" si="8"/>
+        <v>7550.0722215434771</v>
       </c>
       <c r="V7" s="4">
-        <f>G7*(I7*K7+J7*L7)^C7*(M7)^E7*(N7)^D7*(Q7)^F7</f>
+        <f t="shared" si="2"/>
         <v>350.71351329999999</v>
       </c>
       <c r="W7" s="4">
-        <f>B7*(I7*K7+J7*L7)^C7*(M7)^E7*(N7)^D7*(O7)^F7</f>
-        <v>350.71351330000005</v>
+        <f t="shared" si="3"/>
+        <v>350.71351329999999</v>
       </c>
       <c r="X7" s="2" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -3474,16 +3571,16 @@
         <v>16</v>
       </c>
       <c r="B8" s="18">
-        <f>G8*((1-P8)*$B$15)^F8</f>
-        <v>2.3016772933729475</v>
+        <f t="shared" si="4"/>
+        <v>1.1565687226693031</v>
       </c>
       <c r="C8" s="18">
-        <f t="shared" si="1"/>
-        <v>0.41247834812338074</v>
+        <f t="shared" si="5"/>
+        <v>0.22550368920122116</v>
       </c>
       <c r="D8" s="20">
-        <f t="shared" si="2"/>
-        <v>5.856165187661927E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.24553631079877883</v>
       </c>
       <c r="E8" s="3">
         <v>0.11</v>
@@ -3492,8 +3589,8 @@
         <v>0.41896</v>
       </c>
       <c r="G8" s="15">
-        <f t="shared" si="3"/>
-        <v>0.894256737216094</v>
+        <f t="shared" si="7"/>
+        <v>1.1565687226693031</v>
       </c>
       <c r="H8" s="3">
         <v>0.5</v>
@@ -3524,29 +3621,29 @@
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="0"/>
-        <v>505.97809999999993</v>
+        <v>52.981999999999999</v>
       </c>
       <c r="R8" s="4">
-        <f>(I8*K8+J8*L8)^C8*(M8)^E8*(N8)^D8*(Q8)^F8</f>
-        <v>72.041219829728078</v>
+        <f t="shared" si="1"/>
+        <v>55.702134189928742</v>
       </c>
       <c r="S8" s="3">
         <v>64.423346190000004</v>
       </c>
       <c r="T8" s="7">
-        <f t="shared" si="4"/>
-        <v>58.031998790863859</v>
+        <f t="shared" si="8"/>
+        <v>76.059538750186974</v>
       </c>
       <c r="V8" s="4">
-        <f>G8*(I8*K8+J8*L8)^C8*(M8)^E8*(N8)^D8*(Q8)^F8</f>
+        <f t="shared" si="2"/>
         <v>64.42334618999999</v>
       </c>
       <c r="W8" s="4">
-        <f>B8*(I8*K8+J8*L8)^C8*(M8)^E8*(N8)^D8*(O8)^F8</f>
+        <f t="shared" si="3"/>
         <v>64.42334618999999</v>
       </c>
       <c r="X8" s="2" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -3555,16 +3652,16 @@
         <v>17</v>
       </c>
       <c r="B9" s="18">
-        <f>G9*((1-P9)*$B$15)^F9</f>
-        <v>2.5414456169435033</v>
+        <f t="shared" si="4"/>
+        <v>0.95399558454871813</v>
       </c>
       <c r="C9" s="18">
-        <f t="shared" si="1"/>
-        <v>0.44707630059950759</v>
+        <f t="shared" si="5"/>
+        <v>0.2444185388113185</v>
       </c>
       <c r="D9" s="20">
-        <f t="shared" si="2"/>
-        <v>6.3473699400492467E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.26613146118868153</v>
       </c>
       <c r="E9" s="3">
         <v>0.09</v>
@@ -3573,8 +3670,8 @@
         <v>0.39945000000000003</v>
       </c>
       <c r="G9" s="15">
-        <f t="shared" si="3"/>
-        <v>1.0314663470507353</v>
+        <f t="shared" si="7"/>
+        <v>0.95399558454871813</v>
       </c>
       <c r="H9" s="3">
         <v>0.44486066699027998</v>
@@ -3605,29 +3702,29 @@
       </c>
       <c r="Q9" s="4">
         <f t="shared" si="0"/>
-        <v>5677.6349629999995</v>
+        <v>593.95699999999999</v>
       </c>
       <c r="R9" s="4">
-        <f>(I9*K9+J9*L9)^C9*(M9)^E9*(N9)^D9*(Q9)^F9</f>
-        <v>988.82745415428622</v>
+        <f t="shared" si="1"/>
+        <v>1069.1267952592018</v>
       </c>
       <c r="S9" s="3">
         <v>1019.942242</v>
       </c>
       <c r="T9" s="7">
-        <f t="shared" si="4"/>
-        <v>968.13002268377602</v>
+        <f t="shared" si="8"/>
+        <v>2419.1202793072616</v>
       </c>
       <c r="V9" s="4">
-        <f>G9*(I9*K9+J9*L9)^C9*(M9)^E9*(N9)^D9*(Q9)^F9</f>
-        <v>1019.9422420000001</v>
+        <f t="shared" si="2"/>
+        <v>1019.9422419999999</v>
       </c>
       <c r="W9" s="4">
-        <f>B9*(I9*K9+J9*L9)^C9*(M9)^E9*(N9)^D9*(O9)^F9</f>
+        <f t="shared" si="3"/>
         <v>1019.9422419999999</v>
       </c>
       <c r="X9" s="2" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -3636,16 +3733,16 @@
         <v>18</v>
       </c>
       <c r="B10" s="18">
-        <f>G10*((1-P10)*$B$15)^F10</f>
-        <v>0.50806196264562964</v>
+        <f t="shared" si="4"/>
+        <v>0.38118430489918154</v>
       </c>
       <c r="C10" s="18">
-        <f t="shared" si="1"/>
-        <v>0.2780183227447609</v>
+        <f t="shared" si="5"/>
+        <v>0.15199381429283226</v>
       </c>
       <c r="D10" s="20">
-        <f t="shared" si="2"/>
-        <v>3.947167725523916E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.16549618570716776</v>
       </c>
       <c r="E10" s="3">
         <v>0.1</v>
@@ -3654,8 +3751,8 @@
         <v>0.58250999999999997</v>
       </c>
       <c r="G10" s="15">
-        <f t="shared" si="3"/>
-        <v>0.15715192462592548</v>
+        <f t="shared" si="7"/>
+        <v>0.38118430489918154</v>
       </c>
       <c r="H10" s="3">
         <v>0.28394982218742398</v>
@@ -3686,29 +3783,29 @@
       </c>
       <c r="Q10" s="4">
         <f t="shared" si="0"/>
-        <v>303.32564000000002</v>
+        <v>40.465000000000003</v>
       </c>
       <c r="R10" s="4">
-        <f>(I10*K10+J10*L10)^C10*(M10)^E10*(N10)^D10*(Q10)^F10</f>
-        <v>79.30732404115858</v>
+        <f t="shared" si="1"/>
+        <v>32.696253360422034</v>
       </c>
       <c r="S10" s="3">
         <v>12.463298610000001</v>
       </c>
       <c r="T10" s="7">
-        <f t="shared" si="4"/>
-        <v>4468.1237358413755</v>
+        <f t="shared" si="8"/>
+        <v>409.37245793262548</v>
       </c>
       <c r="V10" s="4">
-        <f>G10*(I10*K10+J10*L10)^C10*(M10)^E10*(N10)^D10*(Q10)^F10</f>
+        <f t="shared" si="2"/>
         <v>12.463298610000001</v>
       </c>
       <c r="W10" s="4">
-        <f>B10*(I10*K10+J10*L10)^C10*(M10)^E10*(N10)^D10*(O10)^F10</f>
-        <v>12.463298610000008</v>
+        <f t="shared" si="3"/>
+        <v>12.463298610000001</v>
       </c>
       <c r="X10" s="2" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -3717,16 +3814,16 @@
         <v>20</v>
       </c>
       <c r="B11" s="18">
-        <f>G11*((1-P11)*$B$15)^F11</f>
-        <v>1.9477739649845116</v>
+        <f t="shared" si="4"/>
+        <v>1.2297317515282253</v>
       </c>
       <c r="C11" s="18">
-        <f t="shared" si="1"/>
-        <v>0.30977908549619393</v>
+        <f t="shared" si="5"/>
+        <v>0.16935756006246605</v>
       </c>
       <c r="D11" s="20">
-        <f t="shared" si="2"/>
-        <v>4.3980914503806118E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.184402439937534</v>
       </c>
       <c r="E11" s="3">
         <v>0.09</v>
@@ -3735,8 +3832,8 @@
         <v>0.55623999999999996</v>
       </c>
       <c r="G11" s="15">
-        <f t="shared" si="3"/>
-        <v>0.68471918400506127</v>
+        <f t="shared" si="7"/>
+        <v>1.2297317515282253</v>
       </c>
       <c r="H11" s="3">
         <v>0.54299837350845304</v>
@@ -3767,29 +3864,29 @@
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="0"/>
-        <v>816.10380000000009</v>
+        <v>124.596</v>
       </c>
       <c r="R11" s="4">
-        <f>(I11*K11+J11*L11)^C11*(M11)^E11*(N11)^D11*(Q11)^F11</f>
-        <v>392.9692581798775</v>
+        <f t="shared" si="1"/>
+        <v>218.80673526207158</v>
       </c>
       <c r="S11" s="3">
         <v>269.07358979999998</v>
       </c>
       <c r="T11" s="7">
-        <f t="shared" si="4"/>
-        <v>15350.136643296582</v>
+        <f t="shared" si="8"/>
+        <v>2526.7566651372526</v>
       </c>
       <c r="V11" s="4">
-        <f>G11*(I11*K11+J11*L11)^C11*(M11)^E11*(N11)^D11*(Q11)^F11</f>
+        <f t="shared" si="2"/>
         <v>269.07358979999998</v>
       </c>
       <c r="W11" s="4">
-        <f>B11*(I11*K11+J11*L11)^C11*(M11)^E11*(N11)^D11*(O11)^F11</f>
-        <v>269.07358979999992</v>
+        <f t="shared" si="3"/>
+        <v>269.07358979999998</v>
       </c>
       <c r="X11" s="2" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -3798,16 +3895,16 @@
         <v>19</v>
       </c>
       <c r="B12" s="22">
-        <f>G12*((1-P12)*$B$15)^F12</f>
-        <v>3.7966555337952368</v>
+        <f t="shared" si="4"/>
+        <v>2.4517303309627594</v>
       </c>
       <c r="C12" s="22">
-        <f t="shared" si="1"/>
-        <v>0.18779744085118086</v>
+        <f t="shared" si="5"/>
+        <v>0.10266966963759741</v>
       </c>
       <c r="D12" s="23">
-        <f t="shared" si="2"/>
-        <v>2.6662559148819136E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.11179033036240256</v>
       </c>
       <c r="E12" s="3">
         <v>0.13</v>
@@ -3816,8 +3913,8 @@
         <v>0.65554000000000001</v>
       </c>
       <c r="G12" s="15">
-        <f t="shared" si="3"/>
-        <v>1.0943437116932626</v>
+        <f t="shared" si="7"/>
+        <v>2.4517303309627594</v>
       </c>
       <c r="H12" s="3">
         <v>0.51462882757186901</v>
@@ -3848,29 +3945,29 @@
       </c>
       <c r="Q12" s="4">
         <f t="shared" si="0"/>
-        <v>895.16069000000005</v>
+        <v>134.20699999999999</v>
       </c>
       <c r="R12" s="4">
-        <f>(I12*K12+J12*L12)^C12*(M12)^E12*(N12)^D12*(Q12)^F12</f>
-        <v>387.9263561017213</v>
+        <f t="shared" si="1"/>
+        <v>173.15312497410562</v>
       </c>
       <c r="S12" s="3">
         <v>424.52476840000003</v>
       </c>
       <c r="T12" s="7">
-        <f t="shared" si="4"/>
-        <v>1339.4437827547999</v>
+        <f t="shared" si="8"/>
+        <v>63187.703118635</v>
       </c>
       <c r="V12" s="4">
-        <f>G12*(I12*K12+J12*L12)^C12*(M12)^E12*(N12)^D12*(Q12)^F12</f>
-        <v>424.52476840000003</v>
+        <f t="shared" si="2"/>
+        <v>424.52476840000008</v>
       </c>
       <c r="W12" s="4">
-        <f>B12*(I12*K12+J12*L12)^C12*(M12)^E12*(N12)^D12*(O12)^F12</f>
-        <v>424.5247683999998</v>
+        <f t="shared" si="3"/>
+        <v>424.52476840000008</v>
       </c>
       <c r="X12" s="2" t="b">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
     </row>
@@ -3905,7 +4002,7 @@
       </c>
       <c r="B14" s="8">
         <f>SUM(T3:T12)</f>
-        <v>25249.985099922404</v>
+        <v>94018.837264904229</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -3928,7 +4025,7 @@
         <v>25</v>
       </c>
       <c r="B15" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -3950,7 +4047,7 @@
         <v>24</v>
       </c>
       <c r="B16" s="10">
-        <v>0.87567584095486739</v>
+        <v>0.47873575322949463</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -3974,7 +4071,7 @@
         <v>37</v>
       </c>
       <c r="B17" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -3999,7 +4096,7 @@
       </c>
       <c r="B18" s="4">
         <f>CORREL(R3:R12,S3:S12)</f>
-        <v>0.98846103268649155</v>
+        <v>0.95882771354808249</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -4024,7 +4121,7 @@
       </c>
       <c r="B19" s="4">
         <f>CORREL(G3:G12,H3:H12)</f>
-        <v>0.28092970911817089</v>
+        <v>0.14354174592967628</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -4069,7 +4166,7 @@
       </c>
       <c r="B21" s="4">
         <f>AVERAGE(G3:G12)</f>
-        <v>0.90393995062932286</v>
+        <v>1.4302571802111315</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -4094,7 +4191,7 @@
       </c>
       <c r="B22" s="27">
         <f>AVERAGE(B3:B12)</f>
-        <v>2.6363501671477798</v>
+        <v>1.4302571802111315</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>43</v>
@@ -4165,7 +4262,7 @@
   <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4247,7 +4344,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="18">
-        <f>G3*($B$15)^F3</f>
+        <f t="shared" ref="B3:B12" si="0">G3*($B$15)^F3</f>
         <v>2.2575718249024694</v>
       </c>
       <c r="C3" s="18">
@@ -4267,7 +4364,7 @@
         <v>0.29583171017216714</v>
       </c>
       <c r="G3" s="15">
-        <f t="shared" ref="G3:G12" si="0">P3/O3</f>
+        <f t="shared" ref="G3:G12" si="1">P3/O3</f>
         <v>1.0536911243083609</v>
       </c>
       <c r="H3" s="3">
@@ -4289,11 +4386,11 @@
         <v>93.811000000000007</v>
       </c>
       <c r="N3" s="4">
-        <f t="shared" ref="N3:N12" si="1">M3*$B$15</f>
+        <f t="shared" ref="N3:N12" si="2">M3*$B$15</f>
         <v>1232.7943139575846</v>
       </c>
       <c r="O3" s="4">
-        <f>(I3+J3)^C3*(K3)^E3*(L3)^D3*(N3)^F3</f>
+        <f t="shared" ref="O3:O12" si="3">(I3+J3)^C3*(K3)^E3*(L3)^D3*(N3)^F3</f>
         <v>304.08141352648732</v>
       </c>
       <c r="P3" s="3">
@@ -4304,15 +4401,15 @@
         <v>266.55371975484042</v>
       </c>
       <c r="S3" s="4">
-        <f>(I3+J3)^C3*(K3)^E3*(L3)^D3*(N3)^F3*G3</f>
+        <f t="shared" ref="S3:S12" si="4">(I3+J3)^C3*(K3)^E3*(L3)^D3*(N3)^F3*G3</f>
         <v>320.40788650000002</v>
       </c>
       <c r="T3" s="4">
-        <f>(I3+J3)^C3*(K3)^E3*(L3)^D3*(M3)^F3*B3</f>
+        <f t="shared" ref="T3:T12" si="5">(I3+J3)^C3*(K3)^E3*(L3)^D3*(M3)^F3*B3</f>
         <v>320.40788650000002</v>
       </c>
       <c r="U3" s="2" t="b">
-        <f t="shared" ref="U3:U12" si="2">IF(AND(P3=S3,S3=T3),TRUE, FALSE)</f>
+        <f t="shared" ref="U3:U12" si="6">IF(AND(P3=S3,S3=T3),TRUE, FALSE)</f>
         <v>1</v>
       </c>
     </row>
@@ -4321,27 +4418,27 @@
         <v>9</v>
       </c>
       <c r="B4" s="18">
-        <f>G4*($B$15)^F4</f>
+        <f t="shared" si="0"/>
         <v>1.1654550029056105</v>
       </c>
       <c r="C4" s="18">
-        <f t="shared" ref="C4:C12" si="3">$B$16</f>
+        <f t="shared" ref="C4:C12" si="7">$B$16</f>
         <v>8.5164947045431261E-2</v>
       </c>
       <c r="D4" s="18">
-        <f t="shared" ref="D4:D12" si="4">$B$17</f>
+        <f t="shared" ref="D4:D12" si="8">$B$17</f>
         <v>0.39621680741199822</v>
       </c>
       <c r="E4" s="18">
-        <f t="shared" ref="E4:E12" si="5">$B$18</f>
+        <f t="shared" ref="E4:E12" si="9">$B$18</f>
         <v>0</v>
       </c>
       <c r="F4" s="20">
-        <f t="shared" ref="F4:F12" si="6">$B$19</f>
+        <f t="shared" ref="F4:F12" si="10">$B$19</f>
         <v>0.29583171017216714</v>
       </c>
       <c r="G4" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.54396036431552719</v>
       </c>
       <c r="H4" s="3">
@@ -4363,30 +4460,30 @@
         <v>0.622</v>
       </c>
       <c r="N4" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.1738608828561432</v>
       </c>
       <c r="O4" s="4">
-        <f>(I4+J4)^C4*(K4)^E4*(L4)^D4*(N4)^F4</f>
+        <f t="shared" si="3"/>
         <v>7.0563767983902617</v>
       </c>
       <c r="P4" s="3">
         <v>3.8383892940000002</v>
       </c>
       <c r="Q4" s="7">
-        <f t="shared" ref="Q4:Q12" si="7">(P4-O4)^2</f>
+        <f t="shared" ref="Q4:Q12" si="11">(P4-O4)^2</f>
         <v>10.355443578411863</v>
       </c>
       <c r="S4" s="4">
-        <f>(I4+J4)^C4*(K4)^E4*(L4)^D4*(N4)^F4*G4</f>
+        <f t="shared" si="4"/>
         <v>3.8383892940000002</v>
       </c>
       <c r="T4" s="4">
-        <f>(I4+J4)^C4*(K4)^E4*(L4)^D4*(M4)^F4*B4</f>
+        <f t="shared" si="5"/>
         <v>3.8383892939999993</v>
       </c>
       <c r="U4" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4395,27 +4492,27 @@
         <v>13</v>
       </c>
       <c r="B5" s="18">
-        <f>G5*($B$15)^F5</f>
+        <f t="shared" si="0"/>
         <v>1.0659658603685187</v>
       </c>
       <c r="C5" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>8.5164947045431261E-2</v>
       </c>
       <c r="D5" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.39621680741199822</v>
       </c>
       <c r="E5" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F5" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.29583171017216714</v>
       </c>
       <c r="G5" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.49752515224385285</v>
       </c>
       <c r="H5" s="3">
@@ -4437,30 +4534,30 @@
         <v>4.6139999999999999</v>
       </c>
       <c r="N5" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60.633752594048616</v>
       </c>
       <c r="O5" s="4">
-        <f>(I5+J5)^C5*(K5)^E5*(L5)^D5*(N5)^F5</f>
+        <f t="shared" si="3"/>
         <v>28.618449109124253</v>
       </c>
       <c r="P5" s="3">
         <v>14.238398249999999</v>
       </c>
       <c r="Q5" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>206.78586271100016</v>
       </c>
       <c r="S5" s="4">
-        <f>(I5+J5)^C5*(K5)^E5*(L5)^D5*(N5)^F5*G5</f>
+        <f t="shared" si="4"/>
         <v>14.238398249999999</v>
       </c>
       <c r="T5" s="4">
-        <f>(I5+J5)^C5*(K5)^E5*(L5)^D5*(M5)^F5*B5</f>
+        <f t="shared" si="5"/>
         <v>14.238398249999998</v>
       </c>
       <c r="U5" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4469,27 +4566,27 @@
         <v>14</v>
       </c>
       <c r="B6" s="18">
-        <f>G6*($B$15)^F6</f>
+        <f t="shared" si="0"/>
         <v>0.95244785089667816</v>
       </c>
       <c r="C6" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>8.5164947045431261E-2</v>
       </c>
       <c r="D6" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.39621680741199822</v>
       </c>
       <c r="E6" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F6" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.29583171017216714</v>
       </c>
       <c r="G6" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.44454215621678367</v>
       </c>
       <c r="H6" s="3">
@@ -4511,30 +4608,30 @@
         <v>137.09299999999999</v>
       </c>
       <c r="N6" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1801.5741318543362</v>
       </c>
       <c r="O6" s="4">
-        <f>(I6+J6)^C6*(K6)^E6*(L6)^D6*(N6)^F6</f>
+        <f t="shared" si="3"/>
         <v>99.661079765841393</v>
       </c>
       <c r="P6" s="3">
         <v>44.303551290000001</v>
       </c>
       <c r="Q6" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3064.4559589535907</v>
       </c>
       <c r="S6" s="4">
-        <f>(I6+J6)^C6*(K6)^E6*(L6)^D6*(N6)^F6*G6</f>
+        <f t="shared" si="4"/>
         <v>44.303551290000001</v>
       </c>
       <c r="T6" s="4">
-        <f>(I6+J6)^C6*(K6)^E6*(L6)^D6*(M6)^F6*B6</f>
+        <f t="shared" si="5"/>
         <v>44.303551289999994</v>
       </c>
       <c r="U6" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4543,27 +4640,27 @@
         <v>15</v>
       </c>
       <c r="B7" s="18">
-        <f>G7*($B$15)^F7</f>
+        <f t="shared" si="0"/>
         <v>2.5997877515881576</v>
       </c>
       <c r="C7" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>8.5164947045431261E-2</v>
       </c>
       <c r="D7" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.39621680741199822</v>
       </c>
       <c r="E7" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F7" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.29583171017216714</v>
       </c>
       <c r="G7" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2134157809363946</v>
       </c>
       <c r="H7" s="3">
@@ -4585,30 +4682,30 @@
         <v>195.71799999999999</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2571.9802319466858</v>
       </c>
       <c r="O7" s="4">
-        <f>(I7+J7)^C7*(K7)^E7*(L7)^D7*(N7)^F7</f>
+        <f t="shared" si="3"/>
         <v>289.02995890605109</v>
       </c>
       <c r="P7" s="3">
         <v>350.71351329999999</v>
       </c>
       <c r="Q7" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3804.8608826712521</v>
       </c>
       <c r="S7" s="4">
-        <f>(I7+J7)^C7*(K7)^E7*(L7)^D7*(N7)^F7*G7</f>
+        <f t="shared" si="4"/>
         <v>350.71351330000005</v>
       </c>
       <c r="T7" s="4">
-        <f>(I7+J7)^C7*(K7)^E7*(L7)^D7*(M7)^F7*B7</f>
+        <f t="shared" si="5"/>
         <v>350.71351329999987</v>
       </c>
       <c r="U7" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4617,27 +4714,27 @@
         <v>16</v>
       </c>
       <c r="B8" s="18">
-        <f>G8*($B$15)^F8</f>
+        <f t="shared" si="0"/>
         <v>1.4916020840904538</v>
       </c>
       <c r="C8" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>8.5164947045431261E-2</v>
       </c>
       <c r="D8" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.39621680741199822</v>
       </c>
       <c r="E8" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F8" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.29583171017216714</v>
       </c>
       <c r="G8" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.6961851045752947</v>
       </c>
       <c r="H8" s="3">
@@ -4659,30 +4756,30 @@
         <v>52.981999999999999</v>
       </c>
       <c r="N8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>696.24999565190376</v>
       </c>
       <c r="O8" s="4">
-        <f>(I8+J8)^C8*(K8)^E8*(L8)^D8*(N8)^F8</f>
+        <f t="shared" si="3"/>
         <v>92.537668167004583</v>
       </c>
       <c r="P8" s="3">
         <v>64.423346190000004</v>
       </c>
       <c r="Q8" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>790.41510022668263</v>
       </c>
       <c r="S8" s="4">
-        <f>(I8+J8)^C8*(K8)^E8*(L8)^D8*(N8)^F8*G8</f>
+        <f t="shared" si="4"/>
         <v>64.423346190000004</v>
       </c>
       <c r="T8" s="4">
-        <f>(I8+J8)^C8*(K8)^E8*(L8)^D8*(M8)^F8*B8</f>
+        <f t="shared" si="5"/>
         <v>64.423346189999975</v>
       </c>
       <c r="U8" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4691,27 +4788,27 @@
         <v>17</v>
       </c>
       <c r="B9" s="18">
-        <f>G9*($B$15)^F9</f>
+        <f t="shared" si="0"/>
         <v>2.0774985969125548</v>
       </c>
       <c r="C9" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>8.5164947045431261E-2</v>
       </c>
       <c r="D9" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.39621680741199822</v>
       </c>
       <c r="E9" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F9" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.29583171017216714</v>
       </c>
       <c r="G9" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.9696443799410025</v>
       </c>
       <c r="H9" s="3">
@@ -4733,30 +4830,30 @@
         <v>593.95699999999999</v>
       </c>
       <c r="N9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7805.3406565893665</v>
       </c>
       <c r="O9" s="4">
-        <f>(I9+J9)^C9*(K9)^E9*(L9)^D9*(N9)^F9</f>
+        <f t="shared" si="3"/>
         <v>1051.8724834583766</v>
       </c>
       <c r="P9" s="3">
         <v>1019.942242</v>
       </c>
       <c r="Q9" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1019.5403195902318</v>
       </c>
       <c r="S9" s="4">
-        <f>(I9+J9)^C9*(K9)^E9*(L9)^D9*(N9)^F9*G9</f>
+        <f t="shared" si="4"/>
         <v>1019.942242</v>
       </c>
       <c r="T9" s="4">
-        <f>(I9+J9)^C9*(K9)^E9*(L9)^D9*(M9)^F9*B9</f>
+        <f t="shared" si="5"/>
         <v>1019.9422419999999</v>
       </c>
       <c r="U9" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4765,27 +4862,27 @@
         <v>18</v>
       </c>
       <c r="B10" s="18">
-        <f>G10*($B$15)^F10</f>
+        <f t="shared" si="0"/>
         <v>0.55551427803400211</v>
       </c>
       <c r="C10" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>8.5164947045431261E-2</v>
       </c>
       <c r="D10" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.39621680741199822</v>
       </c>
       <c r="E10" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F10" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.29583171017216714</v>
       </c>
       <c r="G10" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.25927877808108396</v>
       </c>
       <c r="H10" s="3">
@@ -4807,30 +4904,30 @@
         <v>40.465000000000003</v>
       </c>
       <c r="N10" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>531.76090132600291</v>
       </c>
       <c r="O10" s="4">
-        <f>(I10+J10)^C10*(K10)^E10*(L10)^D10*(N10)^F10</f>
+        <f t="shared" si="3"/>
         <v>48.06910423691663</v>
       </c>
       <c r="P10" s="3">
         <v>12.463298610000001</v>
       </c>
       <c r="Q10" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1267.7733943417677</v>
       </c>
       <c r="S10" s="4">
-        <f>(I10+J10)^C10*(K10)^E10*(L10)^D10*(N10)^F10*G10</f>
+        <f t="shared" si="4"/>
         <v>12.463298609999999</v>
       </c>
       <c r="T10" s="4">
-        <f>(I10+J10)^C10*(K10)^E10*(L10)^D10*(M10)^F10*B10</f>
+        <f t="shared" si="5"/>
         <v>12.463298609999997</v>
       </c>
       <c r="U10" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4839,27 +4936,27 @@
         <v>20</v>
       </c>
       <c r="B11" s="18">
-        <f>G11*($B$15)^F11</f>
+        <f t="shared" si="0"/>
         <v>1.8736120479923606</v>
       </c>
       <c r="C11" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>8.5164947045431261E-2</v>
       </c>
       <c r="D11" s="18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.39621680741199822</v>
       </c>
       <c r="E11" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F11" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.29583171017216714</v>
       </c>
       <c r="G11" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.8744830900128947</v>
       </c>
       <c r="H11" s="3">
@@ -4881,30 +4978,30 @@
         <v>124.596</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1637.3478626372089</v>
       </c>
       <c r="O11" s="4">
-        <f>(I11+J11)^C11*(K11)^E11*(L11)^D11*(N11)^F11</f>
+        <f t="shared" si="3"/>
         <v>307.69444586519376</v>
       </c>
       <c r="P11" s="3">
         <v>269.07358979999998</v>
       </c>
       <c r="Q11" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1491.5705232084149</v>
       </c>
       <c r="S11" s="4">
-        <f>(I11+J11)^C11*(K11)^E11*(L11)^D11*(N11)^F11*G11</f>
+        <f t="shared" si="4"/>
         <v>269.07358979999998</v>
       </c>
       <c r="T11" s="4">
-        <f>(I11+J11)^C11*(K11)^E11*(L11)^D11*(M11)^F11*B11</f>
+        <f t="shared" si="5"/>
         <v>269.07358979999987</v>
       </c>
       <c r="U11" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -4913,27 +5010,27 @@
         <v>19</v>
       </c>
       <c r="B12" s="22">
-        <f>G12*($B$15)^F12</f>
+        <f t="shared" si="0"/>
         <v>3.1261263286275907</v>
       </c>
       <c r="C12" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>8.5164947045431261E-2</v>
       </c>
       <c r="D12" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.39621680741199822</v>
       </c>
       <c r="E12" s="22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F12" s="23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.29583171017216714</v>
       </c>
       <c r="G12" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.4590771950672619</v>
       </c>
       <c r="H12" s="3">
@@ -4955,30 +5052,30 @@
         <v>134.20699999999999</v>
       </c>
       <c r="N12" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1763.6484686583187</v>
       </c>
       <c r="O12" s="4">
-        <f>(I12+J12)^C12*(K12)^E12*(L12)^D12*(N12)^F12</f>
+        <f t="shared" si="3"/>
         <v>290.95428935165415</v>
       </c>
       <c r="P12" s="3">
         <v>424.52476840000003</v>
       </c>
       <c r="Q12" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>17841.072873204605</v>
       </c>
       <c r="S12" s="4">
-        <f>(I12+J12)^C12*(K12)^E12*(L12)^D12*(N12)^F12*G12</f>
+        <f t="shared" si="4"/>
         <v>424.52476840000003</v>
       </c>
       <c r="T12" s="4">
-        <f>(I12+J12)^C12*(K12)^E12*(L12)^D12*(M12)^F12*B12</f>
+        <f t="shared" si="5"/>
         <v>424.52476839999997</v>
       </c>
       <c r="U12" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -5298,7 +5395,9 @@
   </sheetPr>
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5379,7 +5478,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="18">
-        <f>G3*($B$15)^F3</f>
+        <f t="shared" ref="B3:B12" si="0">G3*($B$15)^F3</f>
         <v>1.4754808874808347</v>
       </c>
       <c r="C3" s="18">
@@ -5397,7 +5496,7 @@
         <v>0.53442999999999996</v>
       </c>
       <c r="G3" s="15">
-        <f t="shared" ref="G3:G12" si="0">P3/O3</f>
+        <f t="shared" ref="G3:G12" si="1">P3/O3</f>
         <v>1.4754808874808347</v>
       </c>
       <c r="H3" s="3">
@@ -5419,11 +5518,11 @@
         <v>93.811000000000007</v>
       </c>
       <c r="N3" s="4">
-        <f t="shared" ref="N3:N12" si="1">M3*$B$15</f>
+        <f t="shared" ref="N3:N12" si="2">M3*$B$15</f>
         <v>93.811000000000007</v>
       </c>
       <c r="O3" s="4">
-        <f>(I3+J3)^C3*(K3)^E3*(L3)^D3*(N3)^F3</f>
+        <f t="shared" ref="O3:O12" si="3">(I3+J3)^C3*(K3)^E3*(L3)^D3*(N3)^F3</f>
         <v>217.15488775123958</v>
       </c>
       <c r="P3" s="3">
@@ -5434,15 +5533,15 @@
         <v>10661.181750611524</v>
       </c>
       <c r="S3" s="4">
-        <f>(I3+J3)^C3*(K3)^E3*(L3)^D3*(N3)^F3*G3</f>
+        <f t="shared" ref="S3:S12" si="4">(I3+J3)^C3*(K3)^E3*(L3)^D3*(N3)^F3*G3</f>
         <v>320.40788650000002</v>
       </c>
       <c r="T3" s="4">
-        <f>(I3+J3)^C3*(K3)^E3*(L3)^D3*(M3)^F3*B3</f>
+        <f t="shared" ref="T3:T12" si="5">(I3+J3)^C3*(K3)^E3*(L3)^D3*(M3)^F3*B3</f>
         <v>320.40788650000002</v>
       </c>
       <c r="U3" s="2" t="b">
-        <f t="shared" ref="U3:U12" si="2">IF(AND(P3=S3,S3=T3),TRUE, FALSE)</f>
+        <f t="shared" ref="U3:U12" si="6">IF(AND(P3=S3,S3=T3),TRUE, FALSE)</f>
         <v>1</v>
       </c>
     </row>
@@ -5451,15 +5550,15 @@
         <v>9</v>
       </c>
       <c r="B4" s="18">
-        <f>G4*($B$15)^F4</f>
+        <f t="shared" si="0"/>
         <v>3.2465802796648728</v>
       </c>
       <c r="C4" s="18">
-        <f t="shared" ref="C4:C12" si="3">$B$16</f>
+        <f t="shared" ref="C4:C12" si="7">$B$16</f>
         <v>0.21445999999999998</v>
       </c>
       <c r="D4" s="20">
-        <f t="shared" ref="D4:D12" si="4">1-C4-E4-F4</f>
+        <f t="shared" ref="D4:D12" si="8">1-C4-E4-F4</f>
         <v>7.1620000000000017E-2</v>
       </c>
       <c r="E4" s="3">
@@ -5469,7 +5568,7 @@
         <v>0.58391999999999999</v>
       </c>
       <c r="G4" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.2465802796648728</v>
       </c>
       <c r="H4" s="3">
@@ -5491,30 +5590,30 @@
         <v>0.622</v>
       </c>
       <c r="N4" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.622</v>
       </c>
       <c r="O4" s="4">
-        <f>(I4+J4)^C4*(K4)^E4*(L4)^D4*(N4)^F4</f>
+        <f t="shared" si="3"/>
         <v>1.1822868875419328</v>
       </c>
       <c r="P4" s="3">
         <v>3.8383892940000002</v>
       </c>
       <c r="Q4" s="7">
-        <f t="shared" ref="Q4:Q12" si="5">(P4-O4)^2</f>
+        <f t="shared" ref="Q4:Q12" si="9">(P4-O4)^2</f>
         <v>7.054879993592337</v>
       </c>
       <c r="S4" s="4">
-        <f>(I4+J4)^C4*(K4)^E4*(L4)^D4*(N4)^F4*G4</f>
+        <f t="shared" si="4"/>
         <v>3.8383892940000002</v>
       </c>
       <c r="T4" s="4">
-        <f>(I4+J4)^C4*(K4)^E4*(L4)^D4*(M4)^F4*B4</f>
+        <f t="shared" si="5"/>
         <v>3.8383892940000002</v>
       </c>
       <c r="U4" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -5523,15 +5622,15 @@
         <v>13</v>
       </c>
       <c r="B5" s="18">
-        <f>G5*($B$15)^F5</f>
+        <f t="shared" si="0"/>
         <v>1.2665611770363692</v>
       </c>
       <c r="C5" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.21445999999999998</v>
       </c>
       <c r="D5" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.24935000000000007</v>
       </c>
       <c r="E5" s="3">
@@ -5541,7 +5640,7 @@
         <v>0.47619</v>
       </c>
       <c r="G5" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2665611770363692</v>
       </c>
       <c r="H5" s="3">
@@ -5563,30 +5662,30 @@
         <v>4.6139999999999999</v>
       </c>
       <c r="N5" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.6139999999999999</v>
       </c>
       <c r="O5" s="4">
-        <f>(I5+J5)^C5*(K5)^E5*(L5)^D5*(N5)^F5</f>
+        <f t="shared" si="3"/>
         <v>11.241776953337917</v>
       </c>
       <c r="P5" s="3">
         <v>14.238398249999999</v>
       </c>
       <c r="Q5" s="7">
+        <f t="shared" si="9"/>
+        <v>8.979739195608742</v>
+      </c>
+      <c r="S5" s="4">
+        <f t="shared" si="4"/>
+        <v>14.238398249999999</v>
+      </c>
+      <c r="T5" s="4">
         <f t="shared" si="5"/>
-        <v>8.979739195608742</v>
-      </c>
-      <c r="S5" s="4">
-        <f>(I5+J5)^C5*(K5)^E5*(L5)^D5*(N5)^F5*G5</f>
         <v>14.238398249999999</v>
       </c>
-      <c r="T5" s="4">
-        <f>(I5+J5)^C5*(K5)^E5*(L5)^D5*(M5)^F5*B5</f>
-        <v>14.238398249999999</v>
-      </c>
       <c r="U5" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -5595,15 +5694,15 @@
         <v>14</v>
       </c>
       <c r="B6" s="18">
-        <f>G6*($B$15)^F6</f>
+        <f t="shared" si="0"/>
         <v>0.52037635835335083</v>
       </c>
       <c r="C6" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.21445999999999998</v>
       </c>
       <c r="D6" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.29742000000000007</v>
       </c>
       <c r="E6" s="3">
@@ -5613,7 +5712,7 @@
         <v>0.39811999999999997</v>
       </c>
       <c r="G6" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.52037635835335083</v>
       </c>
       <c r="H6" s="3">
@@ -5635,30 +5734,30 @@
         <v>137.09299999999999</v>
       </c>
       <c r="N6" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>137.09299999999999</v>
       </c>
       <c r="O6" s="4">
-        <f>(I6+J6)^C6*(K6)^E6*(L6)^D6*(N6)^F6</f>
+        <f t="shared" si="3"/>
         <v>85.137517450238562</v>
       </c>
       <c r="P6" s="3">
         <v>44.303551290000001</v>
       </c>
       <c r="Q6" s="7">
+        <f t="shared" si="9"/>
+        <v>1667.4127923755079</v>
+      </c>
+      <c r="S6" s="4">
+        <f t="shared" si="4"/>
+        <v>44.303551290000001</v>
+      </c>
+      <c r="T6" s="4">
         <f t="shared" si="5"/>
-        <v>1667.4127923755079</v>
-      </c>
-      <c r="S6" s="4">
-        <f>(I6+J6)^C6*(K6)^E6*(L6)^D6*(N6)^F6*G6</f>
         <v>44.303551290000001</v>
       </c>
-      <c r="T6" s="4">
-        <f>(I6+J6)^C6*(K6)^E6*(L6)^D6*(M6)^F6*B6</f>
-        <v>44.303551290000001</v>
-      </c>
       <c r="U6" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -5667,15 +5766,15 @@
         <v>15</v>
       </c>
       <c r="B7" s="18">
-        <f>G7*($B$15)^F7</f>
+        <f t="shared" si="0"/>
         <v>1.0325073212794107</v>
       </c>
       <c r="C7" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.21445999999999998</v>
       </c>
       <c r="D7" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.26826000000000005</v>
       </c>
       <c r="E7" s="3">
@@ -5685,7 +5784,7 @@
         <v>0.42727999999999999</v>
       </c>
       <c r="G7" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0325073212794107</v>
       </c>
       <c r="H7" s="3">
@@ -5707,30 +5806,30 @@
         <v>195.71799999999999</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>195.71799999999999</v>
       </c>
       <c r="O7" s="4">
-        <f>(I7+J7)^C7*(K7)^E7*(L7)^D7*(N7)^F7</f>
+        <f t="shared" si="3"/>
         <v>339.67169633763024</v>
       </c>
       <c r="P7" s="3">
         <v>350.71351329999999</v>
       </c>
       <c r="Q7" s="7">
+        <f t="shared" si="9"/>
+        <v>121.92172183047636</v>
+      </c>
+      <c r="S7" s="4">
+        <f t="shared" si="4"/>
+        <v>350.71351329999999</v>
+      </c>
+      <c r="T7" s="4">
         <f t="shared" si="5"/>
-        <v>121.92172183047636</v>
-      </c>
-      <c r="S7" s="4">
-        <f>(I7+J7)^C7*(K7)^E7*(L7)^D7*(N7)^F7*G7</f>
         <v>350.71351329999999</v>
       </c>
-      <c r="T7" s="4">
-        <f>(I7+J7)^C7*(K7)^E7*(L7)^D7*(M7)^F7*B7</f>
-        <v>350.71351329999999</v>
-      </c>
       <c r="U7" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -5739,15 +5838,15 @@
         <v>16</v>
       </c>
       <c r="B8" s="18">
-        <f>G8*($B$15)^F8</f>
+        <f t="shared" si="0"/>
         <v>0.91328752048039441</v>
       </c>
       <c r="C8" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.21445999999999998</v>
       </c>
       <c r="D8" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.25658000000000003</v>
       </c>
       <c r="E8" s="3">
@@ -5757,7 +5856,7 @@
         <v>0.41896</v>
       </c>
       <c r="G8" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.91328752048039441</v>
       </c>
       <c r="H8" s="3">
@@ -5779,30 +5878,30 @@
         <v>52.981999999999999</v>
       </c>
       <c r="N8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52.981999999999999</v>
       </c>
       <c r="O8" s="4">
-        <f>(I8+J8)^C8*(K8)^E8*(L8)^D8*(N8)^F8</f>
+        <f t="shared" si="3"/>
         <v>70.540048719939762</v>
       </c>
       <c r="P8" s="3">
         <v>64.423346190000004</v>
       </c>
       <c r="Q8" s="7">
+        <f t="shared" si="9"/>
+        <v>37.414049839771437</v>
+      </c>
+      <c r="S8" s="4">
+        <f t="shared" si="4"/>
+        <v>64.423346190000004</v>
+      </c>
+      <c r="T8" s="4">
         <f t="shared" si="5"/>
-        <v>37.414049839771437</v>
-      </c>
-      <c r="S8" s="4">
-        <f>(I8+J8)^C8*(K8)^E8*(L8)^D8*(N8)^F8*G8</f>
         <v>64.423346190000004</v>
       </c>
-      <c r="T8" s="4">
-        <f>(I8+J8)^C8*(K8)^E8*(L8)^D8*(M8)^F8*B8</f>
-        <v>64.423346190000004</v>
-      </c>
       <c r="U8" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -5811,15 +5910,15 @@
         <v>17</v>
       </c>
       <c r="B9" s="18">
-        <f>G9*($B$15)^F9</f>
+        <f t="shared" si="0"/>
         <v>0.70461230068887282</v>
       </c>
       <c r="C9" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.21445999999999998</v>
       </c>
       <c r="D9" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.29609000000000002</v>
       </c>
       <c r="E9" s="3">
@@ -5829,7 +5928,7 @@
         <v>0.39945000000000003</v>
       </c>
       <c r="G9" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.70461230068887282</v>
       </c>
       <c r="H9" s="3">
@@ -5851,30 +5950,30 @@
         <v>593.95699999999999</v>
       </c>
       <c r="N9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>593.95699999999999</v>
       </c>
       <c r="O9" s="4">
-        <f>(I9+J9)^C9*(K9)^E9*(L9)^D9*(N9)^F9</f>
+        <f t="shared" si="3"/>
         <v>1447.5226177613433</v>
       </c>
       <c r="P9" s="3">
         <v>1019.942242</v>
       </c>
       <c r="Q9" s="7">
+        <f t="shared" si="9"/>
+        <v>182824.97773621159</v>
+      </c>
+      <c r="S9" s="4">
+        <f t="shared" si="4"/>
+        <v>1019.942242</v>
+      </c>
+      <c r="T9" s="4">
         <f t="shared" si="5"/>
-        <v>182824.97773621159</v>
-      </c>
-      <c r="S9" s="4">
-        <f>(I9+J9)^C9*(K9)^E9*(L9)^D9*(N9)^F9*G9</f>
         <v>1019.942242</v>
       </c>
-      <c r="T9" s="4">
-        <f>(I9+J9)^C9*(K9)^E9*(L9)^D9*(M9)^F9*B9</f>
-        <v>1019.942242</v>
-      </c>
       <c r="U9" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -5883,15 +5982,15 @@
         <v>18</v>
       </c>
       <c r="B10" s="18">
-        <f>G10*($B$15)^F10</f>
+        <f t="shared" si="0"/>
         <v>0.39981253396887584</v>
       </c>
       <c r="C10" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.21445999999999998</v>
       </c>
       <c r="D10" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.10303000000000007</v>
       </c>
       <c r="E10" s="3">
@@ -5901,7 +6000,7 @@
         <v>0.58250999999999997</v>
       </c>
       <c r="G10" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.39981253396887584</v>
       </c>
       <c r="H10" s="3">
@@ -5923,30 +6022,30 @@
         <v>40.465000000000003</v>
       </c>
       <c r="N10" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40.465000000000003</v>
       </c>
       <c r="O10" s="4">
-        <f>(I10+J10)^C10*(K10)^E10*(L10)^D10*(N10)^F10</f>
+        <f t="shared" si="3"/>
         <v>31.172856154055015</v>
       </c>
       <c r="P10" s="3">
         <v>12.463298610000001</v>
       </c>
       <c r="Q10" s="7">
+        <f t="shared" si="9"/>
+        <v>350.04754349430596</v>
+      </c>
+      <c r="S10" s="4">
+        <f t="shared" si="4"/>
+        <v>12.463298610000001</v>
+      </c>
+      <c r="T10" s="4">
         <f t="shared" si="5"/>
-        <v>350.04754349430596</v>
-      </c>
-      <c r="S10" s="4">
-        <f>(I10+J10)^C10*(K10)^E10*(L10)^D10*(N10)^F10*G10</f>
         <v>12.463298610000001</v>
       </c>
-      <c r="T10" s="4">
-        <f>(I10+J10)^C10*(K10)^E10*(L10)^D10*(M10)^F10*B10</f>
-        <v>12.463298610000001</v>
-      </c>
       <c r="U10" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -5955,15 +6054,15 @@
         <v>20</v>
       </c>
       <c r="B11" s="18">
-        <f>G11*($B$15)^F11</f>
+        <f t="shared" si="0"/>
         <v>1.2117766205804499</v>
       </c>
       <c r="C11" s="18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.21445999999999998</v>
       </c>
       <c r="D11" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.13930000000000009</v>
       </c>
       <c r="E11" s="3">
@@ -5973,7 +6072,7 @@
         <v>0.55623999999999996</v>
       </c>
       <c r="G11" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2117766205804499</v>
       </c>
       <c r="H11" s="3">
@@ -5995,30 +6094,30 @@
         <v>124.596</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>124.596</v>
       </c>
       <c r="O11" s="4">
-        <f>(I11+J11)^C11*(K11)^E11*(L11)^D11*(N11)^F11</f>
+        <f t="shared" si="3"/>
         <v>222.04883740958113</v>
       </c>
       <c r="P11" s="3">
         <v>269.07358979999998</v>
       </c>
       <c r="Q11" s="7">
+        <f t="shared" si="9"/>
+        <v>2211.3273373802035</v>
+      </c>
+      <c r="S11" s="4">
+        <f t="shared" si="4"/>
+        <v>269.07358979999998</v>
+      </c>
+      <c r="T11" s="4">
         <f t="shared" si="5"/>
-        <v>2211.3273373802035</v>
-      </c>
-      <c r="S11" s="4">
-        <f>(I11+J11)^C11*(K11)^E11*(L11)^D11*(N11)^F11*G11</f>
         <v>269.07358979999998</v>
       </c>
-      <c r="T11" s="4">
-        <f>(I11+J11)^C11*(K11)^E11*(L11)^D11*(M11)^F11*B11</f>
-        <v>269.07358979999998</v>
-      </c>
       <c r="U11" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -6027,15 +6126,15 @@
         <v>19</v>
       </c>
       <c r="B12" s="22">
-        <f>G12*($B$15)^F12</f>
+        <f t="shared" si="0"/>
         <v>3.3673960653554951</v>
       </c>
       <c r="C12" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.21445999999999998</v>
       </c>
       <c r="D12" s="23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="E12" s="3">
@@ -6045,7 +6144,7 @@
         <v>0.65554000000000001</v>
       </c>
       <c r="G12" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.3673960653554951</v>
       </c>
       <c r="H12" s="3">
@@ -6067,30 +6166,30 @@
         <v>134.20699999999999</v>
       </c>
       <c r="N12" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>134.20699999999999</v>
       </c>
       <c r="O12" s="4">
-        <f>(I12+J12)^C12*(K12)^E12*(L12)^D12*(N12)^F12</f>
+        <f t="shared" si="3"/>
         <v>126.06915259170235</v>
       </c>
       <c r="P12" s="3">
         <v>424.52476840000003</v>
       </c>
       <c r="Q12" s="7">
+        <f t="shared" si="9"/>
+        <v>89075.7546075102</v>
+      </c>
+      <c r="S12" s="4">
+        <f t="shared" si="4"/>
+        <v>424.52476840000003</v>
+      </c>
+      <c r="T12" s="4">
         <f t="shared" si="5"/>
-        <v>89075.7546075102</v>
-      </c>
-      <c r="S12" s="4">
-        <f>(I12+J12)^C12*(K12)^E12*(L12)^D12*(N12)^F12*G12</f>
         <v>424.52476840000003</v>
       </c>
-      <c r="T12" s="4">
-        <f>(I12+J12)^C12*(K12)^E12*(L12)^D12*(M12)^F12*B12</f>
-        <v>424.52476840000003</v>
-      </c>
       <c r="U12" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -6309,7 +6408,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6391,7 +6490,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="18">
-        <f>G3*($B$15)^F3</f>
+        <f t="shared" ref="B3:B12" si="0">G3*($B$15)^F3</f>
         <v>1.3463625212068226</v>
       </c>
       <c r="C3" s="18">
@@ -6408,7 +6507,7 @@
         <v>0.53442999999999996</v>
       </c>
       <c r="G3" s="15">
-        <f t="shared" ref="G3:G12" si="0">P3/O3</f>
+        <f t="shared" ref="G3:G12" si="1">P3/O3</f>
         <v>1.0000007977043879</v>
       </c>
       <c r="H3" s="3">
@@ -6430,11 +6529,11 @@
         <v>93.811000000000007</v>
       </c>
       <c r="N3" s="4">
-        <f t="shared" ref="N3:N12" si="1">M3*$B$15</f>
+        <f t="shared" ref="N3:N12" si="2">M3*$B$15</f>
         <v>163.65713140686753</v>
       </c>
       <c r="O3" s="4">
-        <f>(I3+J3)^C3*(K3)^E3*(L3)^D3*(N3)^F3</f>
+        <f t="shared" ref="O3:O12" si="3">(I3+J3)^C3*(K3)^E3*(L3)^D3*(N3)^F3</f>
         <v>320.40763090942693</v>
       </c>
       <c r="P3" s="3">
@@ -6445,15 +6544,15 @@
         <v>6.5326541052527348E-8</v>
       </c>
       <c r="S3" s="4">
-        <f>(I3+J3)^C3*(K3)^E3*(L3)^D3*(N3)^F3*G3</f>
+        <f t="shared" ref="S3:S12" si="4">(I3+J3)^C3*(K3)^E3*(L3)^D3*(N3)^F3*G3</f>
         <v>320.40788650000002</v>
       </c>
       <c r="T3" s="4">
-        <f>(I3+J3)^C3*(K3)^E3*(L3)^D3*(M3)^F3*B3</f>
+        <f t="shared" ref="T3:T12" si="5">(I3+J3)^C3*(K3)^E3*(L3)^D3*(M3)^F3*B3</f>
         <v>320.40788649999996</v>
       </c>
       <c r="U3" s="2" t="b">
-        <f t="shared" ref="U3:U12" si="2">IF(AND(P3=S3,S3=T3),TRUE, FALSE)</f>
+        <f t="shared" ref="U3:U12" si="6">IF(AND(P3=S3,S3=T3),TRUE, FALSE)</f>
         <v>1</v>
       </c>
     </row>
@@ -6462,14 +6561,14 @@
         <v>9</v>
       </c>
       <c r="B4" s="18">
-        <f>G4*($B$15)^F4</f>
+        <f t="shared" si="0"/>
         <v>1.6018335965791768</v>
       </c>
       <c r="C4" s="18">
         <v>0</v>
       </c>
       <c r="D4" s="20">
-        <f t="shared" ref="D4:D12" si="3">1-C4-E4-F4</f>
+        <f t="shared" ref="D4:D12" si="7">1-C4-E4-F4</f>
         <v>0.28608</v>
       </c>
       <c r="E4" s="3">
@@ -6479,7 +6578,7 @@
         <v>0.58391999999999999</v>
       </c>
       <c r="G4" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.157430519966546</v>
       </c>
       <c r="H4" s="3">
@@ -6501,30 +6600,30 @@
         <v>0.622</v>
       </c>
       <c r="N4" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0851044731968702</v>
       </c>
       <c r="O4" s="4">
-        <f>(I4+J4)^C4*(K4)^E4*(L4)^D4*(N4)^F4</f>
+        <f t="shared" si="3"/>
         <v>3.3163021259461378</v>
       </c>
       <c r="P4" s="3">
         <v>3.8383892940000002</v>
       </c>
       <c r="Q4" s="7">
-        <f t="shared" ref="Q4:Q12" si="4">(P4-O4)^2</f>
+        <f t="shared" ref="Q4:Q12" si="8">(P4-O4)^2</f>
         <v>0.27257501104650189</v>
       </c>
       <c r="S4" s="4">
-        <f>(I4+J4)^C4*(K4)^E4*(L4)^D4*(N4)^F4*G4</f>
+        <f t="shared" si="4"/>
         <v>3.8383892940000002</v>
       </c>
       <c r="T4" s="4">
-        <f>(I4+J4)^C4*(K4)^E4*(L4)^D4*(M4)^F4*B4</f>
+        <f t="shared" si="5"/>
         <v>3.8383892940000002</v>
       </c>
       <c r="U4" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -6533,14 +6632,14 @@
         <v>13</v>
       </c>
       <c r="B5" s="18">
-        <f>G5*($B$15)^F5</f>
+        <f t="shared" si="0"/>
         <v>1.3035637514389384</v>
       </c>
       <c r="C5" s="18">
         <v>0.22180465740000813</v>
       </c>
       <c r="D5" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.24200534259999185</v>
       </c>
       <c r="E5" s="3">
@@ -6550,7 +6649,7 @@
         <v>0.47619</v>
       </c>
       <c r="G5" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0001061996946308</v>
       </c>
       <c r="H5" s="3">
@@ -6572,30 +6671,30 @@
         <v>4.6139999999999999</v>
       </c>
       <c r="N5" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.0493119603381977</v>
       </c>
       <c r="O5" s="4">
-        <f>(I5+J5)^C5*(K5)^E5*(L5)^D5*(N5)^F5</f>
+        <f t="shared" si="3"/>
         <v>14.236886297022764</v>
       </c>
       <c r="P5" s="3">
         <v>14.238398249999999</v>
       </c>
       <c r="Q5" s="7">
+        <f t="shared" si="8"/>
+        <v>2.2860018053716216E-6</v>
+      </c>
+      <c r="S5" s="4">
         <f t="shared" si="4"/>
-        <v>2.2860018053716216E-6</v>
-      </c>
-      <c r="S5" s="4">
-        <f>(I5+J5)^C5*(K5)^E5*(L5)^D5*(N5)^F5*G5</f>
         <v>14.238398250000001</v>
       </c>
       <c r="T5" s="4">
-        <f>(I5+J5)^C5*(K5)^E5*(L5)^D5*(M5)^F5*B5</f>
+        <f t="shared" si="5"/>
         <v>14.238398250000003</v>
       </c>
       <c r="U5" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -6604,14 +6703,14 @@
         <v>14</v>
       </c>
       <c r="B6" s="18">
-        <f>G6*($B$15)^F6</f>
+        <f t="shared" si="0"/>
         <v>1.1753326126266146</v>
       </c>
       <c r="C6" s="18">
         <v>0.51188</v>
       </c>
       <c r="D6" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E6" s="3">
@@ -6621,7 +6720,7 @@
         <v>0.39811999999999997</v>
       </c>
       <c r="G6" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.94176528996208986</v>
       </c>
       <c r="H6" s="3">
@@ -6643,30 +6742,30 @@
         <v>137.09299999999999</v>
       </c>
       <c r="N6" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>239.16435296459571</v>
       </c>
       <c r="O6" s="4">
-        <f>(I6+J6)^C6*(K6)^E6*(L6)^D6*(N6)^F6</f>
+        <f t="shared" si="3"/>
         <v>47.043092118826564</v>
       </c>
       <c r="P6" s="3">
         <v>44.303551290000001</v>
       </c>
       <c r="Q6" s="7">
+        <f t="shared" si="8"/>
+        <v>7.5050839528077304</v>
+      </c>
+      <c r="S6" s="4">
         <f t="shared" si="4"/>
-        <v>7.5050839528077304</v>
-      </c>
-      <c r="S6" s="4">
-        <f>(I6+J6)^C6*(K6)^E6*(L6)^D6*(N6)^F6*G6</f>
         <v>44.303551290000001</v>
       </c>
       <c r="T6" s="4">
-        <f>(I6+J6)^C6*(K6)^E6*(L6)^D6*(M6)^F6*B6</f>
+        <f t="shared" si="5"/>
         <v>44.303551290000009</v>
       </c>
       <c r="U6" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -6675,14 +6774,14 @@
         <v>15</v>
       </c>
       <c r="B7" s="18">
-        <f>G7*($B$15)^F7</f>
+        <f t="shared" si="0"/>
         <v>1.2684279430157581</v>
       </c>
       <c r="C7" s="18">
         <v>0.32460421168686593</v>
       </c>
       <c r="D7" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.15811578831313411</v>
       </c>
       <c r="E7" s="3">
@@ -6692,7 +6791,7 @@
         <v>0.42727999999999999</v>
       </c>
       <c r="G7" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.000000623710372</v>
       </c>
       <c r="H7" s="3">
@@ -6714,30 +6813,30 @@
         <v>195.71799999999999</v>
       </c>
       <c r="N7" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>341.43806637483124</v>
       </c>
       <c r="O7" s="4">
-        <f>(I7+J7)^C7*(K7)^E7*(L7)^D7*(N7)^F7</f>
+        <f t="shared" si="3"/>
         <v>350.71329455648055</v>
       </c>
       <c r="P7" s="3">
         <v>350.71351329999999</v>
       </c>
       <c r="Q7" s="7">
+        <f t="shared" si="8"/>
+        <v>4.7848727297027299E-8</v>
+      </c>
+      <c r="S7" s="4">
         <f t="shared" si="4"/>
-        <v>4.7848727297027299E-8</v>
-      </c>
-      <c r="S7" s="4">
-        <f>(I7+J7)^C7*(K7)^E7*(L7)^D7*(N7)^F7*G7</f>
         <v>350.71351329999999</v>
       </c>
       <c r="T7" s="4">
-        <f>(I7+J7)^C7*(K7)^E7*(L7)^D7*(M7)^F7*B7</f>
+        <f t="shared" si="5"/>
         <v>350.71351330000005</v>
       </c>
       <c r="U7" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -6746,14 +6845,14 @@
         <v>16</v>
       </c>
       <c r="B8" s="18">
-        <f>G8*($B$15)^F8</f>
+        <f t="shared" si="0"/>
         <v>1.2624710519849089</v>
       </c>
       <c r="C8" s="18">
         <v>0.33139086012666097</v>
       </c>
       <c r="D8" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.13964913987333905</v>
       </c>
       <c r="E8" s="3">
@@ -6763,7 +6862,7 @@
         <v>0.41896</v>
       </c>
       <c r="G8" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.9999232947917166</v>
       </c>
       <c r="H8" s="3">
@@ -6785,30 +6884,30 @@
         <v>52.981999999999999</v>
       </c>
       <c r="N8" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>92.429268808547548</v>
       </c>
       <c r="O8" s="4">
-        <f>(I8+J8)^C8*(K8)^E8*(L8)^D8*(N8)^F8</f>
+        <f t="shared" si="3"/>
         <v>64.42828817526383</v>
       </c>
       <c r="P8" s="3">
         <v>64.423346190000004</v>
       </c>
       <c r="Q8" s="7">
+        <f t="shared" si="8"/>
+        <v>2.4423218347879362E-5</v>
+      </c>
+      <c r="S8" s="4">
         <f t="shared" si="4"/>
-        <v>2.4423218347879362E-5</v>
-      </c>
-      <c r="S8" s="4">
-        <f>(I8+J8)^C8*(K8)^E8*(L8)^D8*(N8)^F8*G8</f>
         <v>64.423346190000004</v>
       </c>
       <c r="T8" s="4">
-        <f>(I8+J8)^C8*(K8)^E8*(L8)^D8*(M8)^F8*B8</f>
+        <f t="shared" si="5"/>
         <v>64.423346190000018</v>
       </c>
       <c r="U8" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -6817,14 +6916,14 @@
         <v>17</v>
       </c>
       <c r="B9" s="18">
-        <f>G9*($B$15)^F9</f>
+        <f t="shared" si="0"/>
         <v>1.2489317427155628</v>
       </c>
       <c r="C9" s="18">
         <v>0.35415762393642547</v>
       </c>
       <c r="D9" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.15639237606357453</v>
       </c>
       <c r="E9" s="3">
@@ -6834,7 +6933,7 @@
         <v>0.39945000000000003</v>
       </c>
       <c r="G9" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.99999806750201892</v>
       </c>
       <c r="H9" s="3">
@@ -6856,30 +6955,30 @@
         <v>593.95699999999999</v>
       </c>
       <c r="N9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1036.1823112324653</v>
       </c>
       <c r="O9" s="4">
-        <f>(I9+J9)^C9*(K9)^E9*(L9)^D9*(N9)^F9</f>
+        <f t="shared" si="3"/>
         <v>1019.9442130401325</v>
       </c>
       <c r="P9" s="3">
         <v>1019.942242</v>
       </c>
       <c r="Q9" s="7">
+        <f t="shared" si="8"/>
+        <v>3.8849992039367403E-6</v>
+      </c>
+      <c r="S9" s="4">
         <f t="shared" si="4"/>
-        <v>3.8849992039367403E-6</v>
-      </c>
-      <c r="S9" s="4">
-        <f>(I9+J9)^C9*(K9)^E9*(L9)^D9*(N9)^F9*G9</f>
         <v>1019.942242</v>
       </c>
       <c r="T9" s="4">
-        <f>(I9+J9)^C9*(K9)^E9*(L9)^D9*(M9)^F9*B9</f>
+        <f t="shared" si="5"/>
         <v>1019.9422419999999</v>
       </c>
       <c r="U9" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -6888,14 +6987,14 @@
         <v>18</v>
       </c>
       <c r="B10" s="18">
-        <f>G10*($B$15)^F10</f>
+        <f t="shared" si="0"/>
         <v>0.48318275544128692</v>
       </c>
       <c r="C10" s="18">
         <v>0.31749000000000005</v>
       </c>
       <c r="D10" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="E10" s="3">
@@ -6905,7 +7004,7 @@
         <v>0.58250999999999997</v>
       </c>
       <c r="G10" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.34940549305580648</v>
       </c>
       <c r="H10" s="3">
@@ -6927,30 +7026,30 @@
         <v>40.465000000000003</v>
       </c>
       <c r="N10" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70.592849691175815</v>
       </c>
       <c r="O10" s="4">
-        <f>(I10+J10)^C10*(K10)^E10*(L10)^D10*(N10)^F10</f>
+        <f t="shared" si="3"/>
         <v>35.670013373285414</v>
       </c>
       <c r="P10" s="3">
         <v>12.463298610000001</v>
       </c>
       <c r="Q10" s="7">
+        <f t="shared" si="8"/>
+        <v>538.5516101044891</v>
+      </c>
+      <c r="S10" s="4">
         <f t="shared" si="4"/>
-        <v>538.5516101044891</v>
-      </c>
-      <c r="S10" s="4">
-        <f>(I10+J10)^C10*(K10)^E10*(L10)^D10*(N10)^F10*G10</f>
         <v>12.463298610000001</v>
       </c>
       <c r="T10" s="4">
-        <f>(I10+J10)^C10*(K10)^E10*(L10)^D10*(M10)^F10*B10</f>
+        <f t="shared" si="5"/>
         <v>12.463298610000002</v>
       </c>
       <c r="U10" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -6959,14 +7058,14 @@
         <v>20</v>
       </c>
       <c r="B11" s="18">
-        <f>G11*($B$15)^F11</f>
+        <f t="shared" si="0"/>
         <v>1.3628027049420055</v>
       </c>
       <c r="C11" s="18">
         <v>0.26111165687628285</v>
       </c>
       <c r="D11" s="20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>9.2648343123717281E-2</v>
       </c>
       <c r="E11" s="3">
@@ -6976,7 +7075,7 @@
         <v>0.55623999999999996</v>
       </c>
       <c r="G11" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0000005834577261</v>
       </c>
       <c r="H11" s="3">
@@ -6998,30 +7097,30 @@
         <v>124.596</v>
       </c>
       <c r="N11" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>217.36282466629783</v>
       </c>
       <c r="O11" s="4">
-        <f>(I11+J11)^C11*(K11)^E11*(L11)^D11*(N11)^F11</f>
+        <f t="shared" si="3"/>
         <v>269.07343280702673</v>
       </c>
       <c r="P11" s="3">
         <v>269.07358979999998</v>
       </c>
       <c r="Q11" s="7">
+        <f t="shared" si="8"/>
+        <v>2.4646793648446939E-8</v>
+      </c>
+      <c r="S11" s="4">
         <f t="shared" si="4"/>
-        <v>2.4646793648446939E-8</v>
-      </c>
-      <c r="S11" s="4">
-        <f>(I11+J11)^C11*(K11)^E11*(L11)^D11*(N11)^F11*G11</f>
         <v>269.07358979999998</v>
       </c>
       <c r="T11" s="4">
-        <f>(I11+J11)^C11*(K11)^E11*(L11)^D11*(M11)^F11*B11</f>
+        <f t="shared" si="5"/>
         <v>269.07358979999992</v>
       </c>
       <c r="U11" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>
@@ -7030,14 +7129,14 @@
         <v>19</v>
       </c>
       <c r="B12" s="22">
-        <f>G12*($B$15)^F12</f>
+        <f t="shared" si="0"/>
         <v>1.4467933021799875</v>
       </c>
       <c r="C12" s="22">
         <v>0</v>
       </c>
       <c r="D12" s="23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.21445999999999998</v>
       </c>
       <c r="E12" s="3">
@@ -7047,7 +7146,7 @@
         <v>0.65554000000000001</v>
       </c>
       <c r="G12" s="15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.0045575359088108</v>
       </c>
       <c r="H12" s="3">
@@ -7069,30 +7168,30 @@
         <v>134.20699999999999</v>
       </c>
       <c r="N12" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>234.12960777223853</v>
       </c>
       <c r="O12" s="4">
-        <f>(I12+J12)^C12*(K12)^E12*(L12)^D12*(N12)^F12</f>
+        <f t="shared" si="3"/>
         <v>422.59875937911079</v>
       </c>
       <c r="P12" s="3">
         <v>424.52476840000003</v>
       </c>
       <c r="Q12" s="7">
+        <f t="shared" si="8"/>
+        <v>3.7095107485467262</v>
+      </c>
+      <c r="S12" s="4">
         <f t="shared" si="4"/>
-        <v>3.7095107485467262</v>
-      </c>
-      <c r="S12" s="4">
-        <f>(I12+J12)^C12*(K12)^E12*(L12)^D12*(N12)^F12*G12</f>
         <v>424.52476839999997</v>
       </c>
       <c r="T12" s="4">
-        <f>(I12+J12)^C12*(K12)^E12*(L12)^D12*(M12)^F12*B12</f>
+        <f t="shared" si="5"/>
         <v>424.52476839999986</v>
       </c>
       <c r="U12" s="2" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
     </row>

</xml_diff>